<commit_message>
append : rabal case, excel data change
</commit_message>
<xml_diff>
--- a/test/scenarios/Rebalance_Test.xlsx
+++ b/test/scenarios/Rebalance_Test.xlsx
@@ -1679,88 +1679,97 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1775,16 +1784,7 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1793,40 +1793,40 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2991,8 +2991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N31" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N7" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -3008,15 +3008,16 @@
     <col min="9" max="9" width="122.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="47.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="65" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="29" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="25.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.33203125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="25.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="30.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="31.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="25.21875" style="95" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16.33203125" style="2" customWidth="1"/>
@@ -3024,32 +3025,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27.6" customHeight="1">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="139"/>
-      <c r="O1" s="139"/>
-      <c r="P1" s="139"/>
-      <c r="Q1" s="139"/>
-      <c r="R1" s="139"/>
-      <c r="S1" s="139"/>
-      <c r="T1" s="139"/>
-      <c r="U1" s="139"/>
-      <c r="V1" s="139"/>
-      <c r="W1" s="139"/>
-      <c r="X1" s="141"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="98"/>
+      <c r="V1" s="98"/>
+      <c r="W1" s="98"/>
+      <c r="X1" s="100"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
@@ -3147,65 +3148,65 @@
       <c r="Z4" s="21"/>
     </row>
     <row r="5" spans="1:26" ht="9.4499999999999993" customHeight="1">
-      <c r="A5" s="135"/>
-      <c r="B5" s="142" t="s">
+      <c r="A5" s="121"/>
+      <c r="B5" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="120"/>
-      <c r="J5" s="120"/>
-      <c r="K5" s="120"/>
-      <c r="L5" s="120"/>
-      <c r="M5" s="120"/>
-      <c r="N5" s="120"/>
-      <c r="O5" s="120"/>
-      <c r="P5" s="120"/>
-      <c r="Q5" s="120"/>
-      <c r="R5" s="120"/>
-      <c r="S5" s="120"/>
-      <c r="T5" s="120"/>
-      <c r="U5" s="120"/>
-      <c r="V5" s="120"/>
-      <c r="W5" s="120"/>
-      <c r="X5" s="120"/>
-      <c r="Y5" s="143"/>
-      <c r="Z5" s="144"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="111"/>
+      <c r="N5" s="111"/>
+      <c r="O5" s="111"/>
+      <c r="P5" s="111"/>
+      <c r="Q5" s="111"/>
+      <c r="R5" s="111"/>
+      <c r="S5" s="111"/>
+      <c r="T5" s="111"/>
+      <c r="U5" s="111"/>
+      <c r="V5" s="111"/>
+      <c r="W5" s="111"/>
+      <c r="X5" s="111"/>
+      <c r="Y5" s="112"/>
+      <c r="Z5" s="113"/>
     </row>
     <row r="6" spans="1:26" ht="21.9" customHeight="1">
-      <c r="A6" s="136"/>
-      <c r="B6" s="145"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
-      <c r="G6" s="111"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="111"/>
-      <c r="M6" s="111"/>
-      <c r="N6" s="111"/>
-      <c r="O6" s="111"/>
-      <c r="P6" s="111"/>
-      <c r="Q6" s="111"/>
-      <c r="R6" s="111"/>
-      <c r="S6" s="111"/>
-      <c r="T6" s="111"/>
-      <c r="U6" s="111"/>
-      <c r="V6" s="103"/>
-      <c r="W6" s="103"/>
-      <c r="X6" s="103"/>
-      <c r="Y6" s="106"/>
-      <c r="Z6" s="134"/>
+      <c r="A6" s="122"/>
+      <c r="B6" s="114"/>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="115"/>
+      <c r="M6" s="115"/>
+      <c r="N6" s="115"/>
+      <c r="O6" s="115"/>
+      <c r="P6" s="115"/>
+      <c r="Q6" s="115"/>
+      <c r="R6" s="115"/>
+      <c r="S6" s="115"/>
+      <c r="T6" s="115"/>
+      <c r="U6" s="115"/>
+      <c r="V6" s="108"/>
+      <c r="W6" s="108"/>
+      <c r="X6" s="108"/>
+      <c r="Y6" s="116"/>
+      <c r="Z6" s="117"/>
     </row>
     <row r="7" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A7" s="100"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="22" t="s">
         <v>4</v>
       </c>
@@ -3217,23 +3218,23 @@
         <f>B9/0.81</f>
         <v>3778.2175195446539</v>
       </c>
-      <c r="E7" s="102"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="103"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
-      <c r="N7" s="103"/>
-      <c r="O7" s="103"/>
-      <c r="P7" s="103"/>
-      <c r="Q7" s="103"/>
-      <c r="R7" s="103"/>
-      <c r="S7" s="103"/>
-      <c r="T7" s="103"/>
-      <c r="U7" s="104"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="108"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="108"/>
+      <c r="Q7" s="108"/>
+      <c r="R7" s="108"/>
+      <c r="S7" s="108"/>
+      <c r="T7" s="108"/>
+      <c r="U7" s="109"/>
       <c r="V7" s="22" t="s">
         <v>4</v>
       </c>
@@ -3249,7 +3250,7 @@
       <c r="Z7" s="119"/>
     </row>
     <row r="8" spans="1:26" ht="23.85" customHeight="1">
-      <c r="A8" s="100"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="25" t="s">
         <v>5</v>
       </c>
@@ -3327,7 +3328,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="39.9" customHeight="1">
-      <c r="A9" s="101"/>
+      <c r="A9" s="124"/>
       <c r="B9" s="30">
         <f>3060.35619083117</f>
         <v>3060.3561908311699</v>
@@ -3426,7 +3427,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="106" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="34" t="s">
@@ -3468,23 +3469,23 @@
       <c r="N10" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O10" s="129" t="s">
+      <c r="O10" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="P10" s="130"/>
-      <c r="Q10" s="130"/>
-      <c r="R10" s="131"/>
-      <c r="S10" s="108"/>
-      <c r="T10" s="105"/>
-      <c r="U10" s="106"/>
-      <c r="V10" s="106"/>
-      <c r="W10" s="106"/>
-      <c r="X10" s="107"/>
-      <c r="Y10" s="108"/>
-      <c r="Z10" s="109"/>
+      <c r="P10" s="104"/>
+      <c r="Q10" s="104"/>
+      <c r="R10" s="105"/>
+      <c r="S10" s="102"/>
+      <c r="T10" s="134"/>
+      <c r="U10" s="116"/>
+      <c r="V10" s="116"/>
+      <c r="W10" s="116"/>
+      <c r="X10" s="135"/>
+      <c r="Y10" s="102"/>
+      <c r="Z10" s="131"/>
     </row>
     <row r="11" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A11" s="96"/>
+      <c r="A11" s="106"/>
       <c r="B11" s="39">
         <f>SQRT(B9*10^6/10^18)*2^96</f>
         <v>4.3829404691790772E+24</v>
@@ -3536,27 +3537,27 @@
         <f>M11-($B$3*E11)*B11</f>
         <v>1.2889378916075946E+43</v>
       </c>
-      <c r="O11" s="128" t="s">
+      <c r="O11" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="P11" s="108"/>
-      <c r="Q11" s="128" t="s">
+      <c r="P11" s="102"/>
+      <c r="Q11" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="R11" s="108"/>
+      <c r="R11" s="102"/>
       <c r="S11" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="T11" s="110"/>
-      <c r="U11" s="111"/>
-      <c r="V11" s="111"/>
-      <c r="W11" s="111"/>
-      <c r="X11" s="112"/>
-      <c r="Y11" s="108"/>
-      <c r="Z11" s="109"/>
+      <c r="T11" s="136"/>
+      <c r="U11" s="115"/>
+      <c r="V11" s="115"/>
+      <c r="W11" s="115"/>
+      <c r="X11" s="137"/>
+      <c r="Y11" s="102"/>
+      <c r="Z11" s="131"/>
     </row>
     <row r="12" spans="1:26" ht="20.85" customHeight="1">
-      <c r="A12" s="96" t="s">
+      <c r="A12" s="106" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="34" t="s">
@@ -3617,16 +3618,16 @@
         <f>(P13-Q12)/2*(1-0.0003)</f>
         <v>-0.42613940834773056</v>
       </c>
-      <c r="T12" s="110"/>
-      <c r="U12" s="111"/>
-      <c r="V12" s="111"/>
-      <c r="W12" s="111"/>
-      <c r="X12" s="112"/>
-      <c r="Y12" s="108"/>
-      <c r="Z12" s="109"/>
+      <c r="T12" s="136"/>
+      <c r="U12" s="115"/>
+      <c r="V12" s="115"/>
+      <c r="W12" s="115"/>
+      <c r="X12" s="137"/>
+      <c r="Y12" s="102"/>
+      <c r="Z12" s="131"/>
     </row>
     <row r="13" spans="1:26" ht="30" customHeight="1">
-      <c r="A13" s="97"/>
+      <c r="A13" s="120"/>
       <c r="B13" s="48">
         <f>SQRT(V9*10^6/10^18)*2^96</f>
         <v>4.3972388145443278E+24</v>
@@ -3694,13 +3695,13 @@
         <v>10000.426139408348</v>
       </c>
       <c r="S13" s="56"/>
-      <c r="T13" s="113"/>
-      <c r="U13" s="114"/>
-      <c r="V13" s="114"/>
-      <c r="W13" s="114"/>
-      <c r="X13" s="115"/>
-      <c r="Y13" s="116"/>
-      <c r="Z13" s="117"/>
+      <c r="T13" s="138"/>
+      <c r="U13" s="139"/>
+      <c r="V13" s="139"/>
+      <c r="W13" s="139"/>
+      <c r="X13" s="140"/>
+      <c r="Y13" s="141"/>
+      <c r="Z13" s="142"/>
     </row>
     <row r="14" spans="1:26" ht="21.3" customHeight="1">
       <c r="A14" s="57"/>
@@ -3759,65 +3760,65 @@
       <c r="Z15" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="9.4499999999999993" customHeight="1">
-      <c r="A16" s="98"/>
-      <c r="B16" s="124" t="s">
+      <c r="A16" s="125"/>
+      <c r="B16" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="120"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="120"/>
-      <c r="J16" s="120"/>
-      <c r="K16" s="120"/>
-      <c r="L16" s="120"/>
-      <c r="M16" s="120"/>
-      <c r="N16" s="120"/>
-      <c r="O16" s="120"/>
-      <c r="P16" s="120"/>
-      <c r="Q16" s="120"/>
-      <c r="R16" s="120"/>
-      <c r="S16" s="120"/>
-      <c r="T16" s="120"/>
-      <c r="U16" s="120"/>
-      <c r="V16" s="120"/>
-      <c r="W16" s="120"/>
-      <c r="X16" s="120"/>
-      <c r="Y16" s="125"/>
-      <c r="Z16" s="126"/>
+      <c r="C16" s="111"/>
+      <c r="D16" s="111"/>
+      <c r="E16" s="111"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="111"/>
+      <c r="H16" s="111"/>
+      <c r="I16" s="111"/>
+      <c r="J16" s="111"/>
+      <c r="K16" s="111"/>
+      <c r="L16" s="111"/>
+      <c r="M16" s="111"/>
+      <c r="N16" s="111"/>
+      <c r="O16" s="111"/>
+      <c r="P16" s="111"/>
+      <c r="Q16" s="111"/>
+      <c r="R16" s="111"/>
+      <c r="S16" s="111"/>
+      <c r="T16" s="111"/>
+      <c r="U16" s="111"/>
+      <c r="V16" s="111"/>
+      <c r="W16" s="111"/>
+      <c r="X16" s="111"/>
+      <c r="Y16" s="128"/>
+      <c r="Z16" s="129"/>
     </row>
     <row r="17" spans="1:26" ht="21.9" customHeight="1">
-      <c r="A17" s="99"/>
-      <c r="B17" s="103"/>
-      <c r="C17" s="103"/>
-      <c r="D17" s="103"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="111"/>
-      <c r="H17" s="111"/>
-      <c r="I17" s="111"/>
-      <c r="J17" s="111"/>
-      <c r="K17" s="111"/>
-      <c r="L17" s="111"/>
-      <c r="M17" s="111"/>
-      <c r="N17" s="111"/>
-      <c r="O17" s="111"/>
-      <c r="P17" s="111"/>
-      <c r="Q17" s="111"/>
-      <c r="R17" s="111"/>
-      <c r="S17" s="111"/>
-      <c r="T17" s="111"/>
-      <c r="U17" s="111"/>
-      <c r="V17" s="103"/>
-      <c r="W17" s="103"/>
-      <c r="X17" s="103"/>
-      <c r="Y17" s="120"/>
-      <c r="Z17" s="127"/>
+      <c r="A17" s="126"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="108"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="115"/>
+      <c r="G17" s="115"/>
+      <c r="H17" s="115"/>
+      <c r="I17" s="115"/>
+      <c r="J17" s="115"/>
+      <c r="K17" s="115"/>
+      <c r="L17" s="115"/>
+      <c r="M17" s="115"/>
+      <c r="N17" s="115"/>
+      <c r="O17" s="115"/>
+      <c r="P17" s="115"/>
+      <c r="Q17" s="115"/>
+      <c r="R17" s="115"/>
+      <c r="S17" s="115"/>
+      <c r="T17" s="115"/>
+      <c r="U17" s="115"/>
+      <c r="V17" s="108"/>
+      <c r="W17" s="108"/>
+      <c r="X17" s="108"/>
+      <c r="Y17" s="111"/>
+      <c r="Z17" s="130"/>
     </row>
     <row r="18" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A18" s="100"/>
+      <c r="A18" s="123"/>
       <c r="B18" s="22" t="s">
         <v>4</v>
       </c>
@@ -3829,23 +3830,23 @@
         <f>B20/0.81</f>
         <v>3778.2175195446539</v>
       </c>
-      <c r="E18" s="102"/>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="103"/>
-      <c r="I18" s="103"/>
-      <c r="J18" s="103"/>
-      <c r="K18" s="103"/>
-      <c r="L18" s="103"/>
-      <c r="M18" s="103"/>
-      <c r="N18" s="103"/>
-      <c r="O18" s="103"/>
-      <c r="P18" s="103"/>
-      <c r="Q18" s="103"/>
-      <c r="R18" s="103"/>
-      <c r="S18" s="103"/>
-      <c r="T18" s="103"/>
-      <c r="U18" s="104"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="108"/>
+      <c r="K18" s="108"/>
+      <c r="L18" s="108"/>
+      <c r="M18" s="108"/>
+      <c r="N18" s="108"/>
+      <c r="O18" s="108"/>
+      <c r="P18" s="108"/>
+      <c r="Q18" s="108"/>
+      <c r="R18" s="108"/>
+      <c r="S18" s="108"/>
+      <c r="T18" s="108"/>
+      <c r="U18" s="109"/>
       <c r="V18" s="22" t="s">
         <v>4</v>
       </c>
@@ -3861,7 +3862,7 @@
       <c r="Z18" s="119"/>
     </row>
     <row r="19" spans="1:26" ht="23.85" customHeight="1">
-      <c r="A19" s="100"/>
+      <c r="A19" s="123"/>
       <c r="B19" s="25" t="s">
         <v>5</v>
       </c>
@@ -3939,7 +3940,7 @@
       </c>
     </row>
     <row r="20" spans="1:26" ht="40.5" customHeight="1">
-      <c r="A20" s="101"/>
+      <c r="A20" s="124"/>
       <c r="B20" s="30">
         <f t="shared" ref="B20:B53" si="1">3060.35619083117</f>
         <v>3060.3561908311699</v>
@@ -3981,14 +3982,15 @@
         <v>3.26787207467537</v>
       </c>
       <c r="L20" s="31">
-        <f>F20+J20+N20</f>
-        <v>15112.241467</v>
+        <f>15112.232914</f>
+        <v>15112.232914</v>
       </c>
       <c r="M20" s="31">
         <v>0</v>
       </c>
       <c r="N20" s="31">
-        <v>5112.2414669999998</v>
+        <f>L20-F22/1000000</f>
+        <v>5112.2329140000002</v>
       </c>
       <c r="O20" s="31">
         <v>3060.3561909999999</v>
@@ -3999,23 +4001,23 @@
       </c>
       <c r="Q20" s="31">
         <f>IF(S23&gt;0,S23,0)</f>
-        <v>2554.9277575958281</v>
+        <v>2554.9234823787783</v>
       </c>
       <c r="R20" s="31">
         <f>R23</f>
-        <v>4.1027186082617044</v>
+        <v>4.1027172112945598</v>
       </c>
       <c r="S20" s="31">
         <f>R24</f>
-        <v>12557.313709404172</v>
+        <v>12557.309431621223</v>
       </c>
       <c r="T20" s="31">
         <f>R20*$B$3</f>
-        <v>0.41027186082617045</v>
+        <v>0.41027172112945598</v>
       </c>
       <c r="U20" s="31">
         <f>S20*$B$3</f>
-        <v>1255.7313709404173</v>
+        <v>1255.7309431621225</v>
       </c>
       <c r="V20" s="31">
         <v>3060.3561909999999</v>
@@ -4030,15 +4032,15 @@
       </c>
       <c r="Y20" s="32">
         <f>(G24/T20)-1</f>
-        <v>1.3413627060614663E-2</v>
+        <v>1.3413627060614886E-2</v>
       </c>
       <c r="Z20" s="33">
         <f>(H24/U20)-1</f>
-        <v>6.8655601523872622E-3</v>
+        <v>6.8655603162603995E-3</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A21" s="96" t="s">
+      <c r="A21" s="106" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="34" t="s">
@@ -4080,23 +4082,23 @@
       <c r="N21" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O21" s="129" t="s">
+      <c r="O21" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="P21" s="130"/>
-      <c r="Q21" s="130"/>
-      <c r="R21" s="131"/>
-      <c r="S21" s="108"/>
-      <c r="T21" s="105"/>
-      <c r="U21" s="106"/>
-      <c r="V21" s="106"/>
-      <c r="W21" s="106"/>
-      <c r="X21" s="107"/>
-      <c r="Y21" s="108"/>
-      <c r="Z21" s="109"/>
+      <c r="P21" s="104"/>
+      <c r="Q21" s="104"/>
+      <c r="R21" s="105"/>
+      <c r="S21" s="102"/>
+      <c r="T21" s="134"/>
+      <c r="U21" s="116"/>
+      <c r="V21" s="116"/>
+      <c r="W21" s="116"/>
+      <c r="X21" s="135"/>
+      <c r="Y21" s="102"/>
+      <c r="Z21" s="131"/>
     </row>
     <row r="22" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A22" s="96"/>
+      <c r="A22" s="106"/>
       <c r="B22" s="39">
         <f>SQRT(B20*10^6/10^18)*2^96</f>
         <v>4.3829404691790772E+24</v>
@@ -4148,27 +4150,27 @@
         <f>M22-(0.1*E22)*B22</f>
         <v>1.2889378916075946E+43</v>
       </c>
-      <c r="O22" s="128" t="s">
+      <c r="O22" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="P22" s="108"/>
-      <c r="Q22" s="128" t="s">
+      <c r="P22" s="102"/>
+      <c r="Q22" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="R22" s="108"/>
+      <c r="R22" s="102"/>
       <c r="S22" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="T22" s="110"/>
-      <c r="U22" s="111"/>
-      <c r="V22" s="111"/>
-      <c r="W22" s="111"/>
-      <c r="X22" s="112"/>
-      <c r="Y22" s="108"/>
-      <c r="Z22" s="109"/>
+      <c r="T22" s="136"/>
+      <c r="U22" s="115"/>
+      <c r="V22" s="115"/>
+      <c r="W22" s="115"/>
+      <c r="X22" s="137"/>
+      <c r="Y22" s="102"/>
+      <c r="Z22" s="131"/>
     </row>
     <row r="23" spans="1:26" ht="20.85" customHeight="1">
-      <c r="A23" s="96" t="s">
+      <c r="A23" s="106" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="34" t="s">
@@ -4223,29 +4225,29 @@
       </c>
       <c r="R23" s="47">
         <f>P23+(S23/O20)</f>
-        <v>4.1027186082617044</v>
+        <v>4.1027172112945598</v>
       </c>
       <c r="S23" s="47">
         <f>(P24-Q23)/2*(1-0.0003)</f>
-        <v>2554.9277575958281</v>
-      </c>
-      <c r="T23" s="110"/>
-      <c r="U23" s="111"/>
-      <c r="V23" s="111"/>
-      <c r="W23" s="111"/>
-      <c r="X23" s="112"/>
-      <c r="Y23" s="108"/>
-      <c r="Z23" s="109"/>
+        <v>2554.9234823787783</v>
+      </c>
+      <c r="T23" s="136"/>
+      <c r="U23" s="115"/>
+      <c r="V23" s="115"/>
+      <c r="W23" s="115"/>
+      <c r="X23" s="137"/>
+      <c r="Y23" s="102"/>
+      <c r="Z23" s="131"/>
     </row>
     <row r="24" spans="1:26" ht="21.3" customHeight="1">
-      <c r="A24" s="97"/>
+      <c r="A24" s="120"/>
       <c r="B24" s="48">
         <f>SQRT(V20*10^6/10^18)*2^96</f>
         <v>4.3829404692999735E+24</v>
       </c>
       <c r="C24" s="49">
         <f>B24-$B$3*F24*POWER(2,96)/L24</f>
-        <v>3.9445928942429745E+24</v>
+        <v>3.9445928943143177E+24</v>
       </c>
       <c r="D24" s="49">
         <f>M24*B24/N24</f>
@@ -4253,66 +4255,66 @@
       </c>
       <c r="E24" s="49">
         <f>R20*10^18</f>
-        <v>4.1027186082617042E+18</v>
+        <v>4.1027172112945597E+18</v>
       </c>
       <c r="F24" s="49">
         <f>S20*10^6</f>
-        <v>12557313709.404173</v>
+        <v>12557309431.621223</v>
       </c>
       <c r="G24" s="50">
         <f>(M24-(M24*B24)/(SQRT(1/(1.0001^X20)*2^96*2^96/10^6)*10^3))/B24/10^18</f>
-        <v>0.41577509456075712</v>
+        <v>0.41577495299020312</v>
       </c>
       <c r="H24" s="50">
         <f>(B24-(SQRT(1/(1.0001^W20)*2^96*2^96)))*L24/POWER(2,96)/10^6</f>
-        <v>1264.3526702028485</v>
+        <v>1264.3522396933965</v>
       </c>
       <c r="I24" s="49">
         <v>9.9999999999999997E+98</v>
       </c>
       <c r="J24" s="49">
         <f>(E24)*(B24*I24)/POWER(2,96)/(I24-B24)</f>
-        <v>226964388061666.72</v>
+        <v>226964310780765.09</v>
       </c>
       <c r="K24" s="49">
         <f>(F24)*POWER(2,96)/(B24-0)</f>
-        <v>226992106846975.69</v>
+        <v>226992029519691.62</v>
       </c>
       <c r="L24" s="49">
         <f>MIN(J24,K24)</f>
-        <v>226964388061666.72</v>
+        <v>226964310780765.09</v>
       </c>
       <c r="M24" s="49">
         <f>L24*POWER(2,96)</f>
-        <v>1.7981971422300287E+43</v>
+        <v>1.7981965299476454E+43</v>
       </c>
       <c r="N24" s="51">
         <f>M24-(0.1*E24)*B24</f>
-        <v>1.618377428007026E+43</v>
+        <v>1.618376876952881E+43</v>
       </c>
       <c r="O24" s="52" t="s">
         <v>49</v>
       </c>
       <c r="P24" s="53">
         <f>L20</f>
-        <v>15112.241467</v>
+        <v>15112.232914</v>
       </c>
       <c r="Q24" s="54">
         <f>P24/O20</f>
-        <v>4.9380662000856619</v>
+        <v>4.9380634053129411</v>
       </c>
       <c r="R24" s="55">
         <f>P24-S23</f>
-        <v>12557.313709404172</v>
+        <v>12557.309431621223</v>
       </c>
       <c r="S24" s="56"/>
-      <c r="T24" s="113"/>
-      <c r="U24" s="114"/>
-      <c r="V24" s="114"/>
-      <c r="W24" s="114"/>
-      <c r="X24" s="115"/>
-      <c r="Y24" s="116"/>
-      <c r="Z24" s="117"/>
+      <c r="T24" s="138"/>
+      <c r="U24" s="139"/>
+      <c r="V24" s="139"/>
+      <c r="W24" s="139"/>
+      <c r="X24" s="140"/>
+      <c r="Y24" s="141"/>
+      <c r="Z24" s="142"/>
     </row>
     <row r="25" spans="1:26" ht="21.3" customHeight="1">
       <c r="A25" s="57"/>
@@ -4371,65 +4373,65 @@
       <c r="Z26" s="59"/>
     </row>
     <row r="27" spans="1:26" ht="9.4499999999999993" customHeight="1">
-      <c r="A27" s="98"/>
-      <c r="B27" s="124" t="s">
+      <c r="A27" s="125"/>
+      <c r="B27" s="127" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="120"/>
-      <c r="D27" s="120"/>
-      <c r="E27" s="120"/>
-      <c r="F27" s="120"/>
-      <c r="G27" s="120"/>
-      <c r="H27" s="120"/>
-      <c r="I27" s="120"/>
-      <c r="J27" s="120"/>
-      <c r="K27" s="120"/>
-      <c r="L27" s="120"/>
-      <c r="M27" s="120"/>
-      <c r="N27" s="120"/>
-      <c r="O27" s="120"/>
-      <c r="P27" s="120"/>
-      <c r="Q27" s="120"/>
-      <c r="R27" s="120"/>
-      <c r="S27" s="120"/>
-      <c r="T27" s="120"/>
-      <c r="U27" s="120"/>
-      <c r="V27" s="120"/>
-      <c r="W27" s="120"/>
-      <c r="X27" s="120"/>
-      <c r="Y27" s="125"/>
-      <c r="Z27" s="126"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="111"/>
+      <c r="H27" s="111"/>
+      <c r="I27" s="111"/>
+      <c r="J27" s="111"/>
+      <c r="K27" s="111"/>
+      <c r="L27" s="111"/>
+      <c r="M27" s="111"/>
+      <c r="N27" s="111"/>
+      <c r="O27" s="111"/>
+      <c r="P27" s="111"/>
+      <c r="Q27" s="111"/>
+      <c r="R27" s="111"/>
+      <c r="S27" s="111"/>
+      <c r="T27" s="111"/>
+      <c r="U27" s="111"/>
+      <c r="V27" s="111"/>
+      <c r="W27" s="111"/>
+      <c r="X27" s="111"/>
+      <c r="Y27" s="128"/>
+      <c r="Z27" s="129"/>
     </row>
     <row r="28" spans="1:26" ht="21.9" customHeight="1">
-      <c r="A28" s="99"/>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="111"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="111"/>
-      <c r="H28" s="111"/>
-      <c r="I28" s="111"/>
-      <c r="J28" s="111"/>
-      <c r="K28" s="111"/>
-      <c r="L28" s="111"/>
-      <c r="M28" s="111"/>
-      <c r="N28" s="111"/>
-      <c r="O28" s="111"/>
-      <c r="P28" s="111"/>
-      <c r="Q28" s="111"/>
-      <c r="R28" s="111"/>
-      <c r="S28" s="111"/>
-      <c r="T28" s="111"/>
-      <c r="U28" s="111"/>
-      <c r="V28" s="103"/>
-      <c r="W28" s="103"/>
-      <c r="X28" s="103"/>
-      <c r="Y28" s="120"/>
-      <c r="Z28" s="127"/>
+      <c r="A28" s="126"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="115"/>
+      <c r="F28" s="115"/>
+      <c r="G28" s="115"/>
+      <c r="H28" s="115"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="115"/>
+      <c r="K28" s="115"/>
+      <c r="L28" s="115"/>
+      <c r="M28" s="115"/>
+      <c r="N28" s="115"/>
+      <c r="O28" s="115"/>
+      <c r="P28" s="115"/>
+      <c r="Q28" s="115"/>
+      <c r="R28" s="115"/>
+      <c r="S28" s="115"/>
+      <c r="T28" s="115"/>
+      <c r="U28" s="115"/>
+      <c r="V28" s="108"/>
+      <c r="W28" s="108"/>
+      <c r="X28" s="108"/>
+      <c r="Y28" s="111"/>
+      <c r="Z28" s="130"/>
     </row>
     <row r="29" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A29" s="100"/>
+      <c r="A29" s="123"/>
       <c r="B29" s="22" t="s">
         <v>4</v>
       </c>
@@ -4441,23 +4443,23 @@
         <f>B31/0.81</f>
         <v>3778.2175195446539</v>
       </c>
-      <c r="E29" s="102"/>
-      <c r="F29" s="103"/>
-      <c r="G29" s="103"/>
-      <c r="H29" s="103"/>
-      <c r="I29" s="103"/>
-      <c r="J29" s="103"/>
-      <c r="K29" s="103"/>
-      <c r="L29" s="103"/>
-      <c r="M29" s="103"/>
-      <c r="N29" s="103"/>
-      <c r="O29" s="103"/>
-      <c r="P29" s="103"/>
-      <c r="Q29" s="103"/>
-      <c r="R29" s="103"/>
-      <c r="S29" s="103"/>
-      <c r="T29" s="103"/>
-      <c r="U29" s="104"/>
+      <c r="E29" s="107"/>
+      <c r="F29" s="108"/>
+      <c r="G29" s="108"/>
+      <c r="H29" s="108"/>
+      <c r="I29" s="108"/>
+      <c r="J29" s="108"/>
+      <c r="K29" s="108"/>
+      <c r="L29" s="108"/>
+      <c r="M29" s="108"/>
+      <c r="N29" s="108"/>
+      <c r="O29" s="108"/>
+      <c r="P29" s="108"/>
+      <c r="Q29" s="108"/>
+      <c r="R29" s="108"/>
+      <c r="S29" s="108"/>
+      <c r="T29" s="108"/>
+      <c r="U29" s="109"/>
       <c r="V29" s="22" t="s">
         <v>4</v>
       </c>
@@ -4473,7 +4475,7 @@
       <c r="Z29" s="119"/>
     </row>
     <row r="30" spans="1:26" ht="23.85" customHeight="1">
-      <c r="A30" s="100"/>
+      <c r="A30" s="123"/>
       <c r="B30" s="25" t="s">
         <v>5</v>
       </c>
@@ -4551,7 +4553,7 @@
       </c>
     </row>
     <row r="31" spans="1:26" ht="40.35" customHeight="1">
-      <c r="A31" s="101"/>
+      <c r="A31" s="124"/>
       <c r="B31" s="30">
         <f t="shared" si="1"/>
         <v>3060.3561908311699</v>
@@ -4651,7 +4653,7 @@
       </c>
     </row>
     <row r="32" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A32" s="96" t="s">
+      <c r="A32" s="106" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="34" t="s">
@@ -4693,23 +4695,23 @@
       <c r="N32" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O32" s="129" t="s">
+      <c r="O32" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="P32" s="130"/>
-      <c r="Q32" s="130"/>
-      <c r="R32" s="131"/>
-      <c r="S32" s="108"/>
-      <c r="T32" s="105"/>
-      <c r="U32" s="106"/>
-      <c r="V32" s="106"/>
-      <c r="W32" s="106"/>
-      <c r="X32" s="107"/>
-      <c r="Y32" s="108"/>
-      <c r="Z32" s="109"/>
+      <c r="P32" s="104"/>
+      <c r="Q32" s="104"/>
+      <c r="R32" s="105"/>
+      <c r="S32" s="102"/>
+      <c r="T32" s="134"/>
+      <c r="U32" s="116"/>
+      <c r="V32" s="116"/>
+      <c r="W32" s="116"/>
+      <c r="X32" s="135"/>
+      <c r="Y32" s="102"/>
+      <c r="Z32" s="131"/>
     </row>
     <row r="33" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A33" s="96"/>
+      <c r="A33" s="106"/>
       <c r="B33" s="39">
         <f>SQRT(B31*10^6/10^18)*2^96</f>
         <v>4.3829404691790772E+24</v>
@@ -4761,27 +4763,27 @@
         <f>M33-(0.1*E33)*B33</f>
         <v>1.5966769901727963E+43</v>
       </c>
-      <c r="O33" s="128" t="s">
+      <c r="O33" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="P33" s="108"/>
-      <c r="Q33" s="128" t="s">
+      <c r="P33" s="102"/>
+      <c r="Q33" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="R33" s="108"/>
+      <c r="R33" s="102"/>
       <c r="S33" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="T33" s="110"/>
-      <c r="U33" s="111"/>
-      <c r="V33" s="111"/>
-      <c r="W33" s="111"/>
-      <c r="X33" s="112"/>
-      <c r="Y33" s="108"/>
-      <c r="Z33" s="109"/>
+      <c r="T33" s="136"/>
+      <c r="U33" s="115"/>
+      <c r="V33" s="115"/>
+      <c r="W33" s="115"/>
+      <c r="X33" s="137"/>
+      <c r="Y33" s="102"/>
+      <c r="Z33" s="131"/>
     </row>
     <row r="34" spans="1:26" ht="20.85" customHeight="1">
-      <c r="A34" s="96" t="s">
+      <c r="A34" s="106" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="34" t="s">
@@ -4842,16 +4844,16 @@
         <f>(P35-Q34)/2*(1-0.0003)</f>
         <v>-726.20415820028688</v>
       </c>
-      <c r="T34" s="110"/>
-      <c r="U34" s="111"/>
-      <c r="V34" s="111"/>
-      <c r="W34" s="111"/>
-      <c r="X34" s="112"/>
-      <c r="Y34" s="108"/>
-      <c r="Z34" s="109"/>
+      <c r="T34" s="136"/>
+      <c r="U34" s="115"/>
+      <c r="V34" s="115"/>
+      <c r="W34" s="115"/>
+      <c r="X34" s="137"/>
+      <c r="Y34" s="102"/>
+      <c r="Z34" s="131"/>
     </row>
     <row r="35" spans="1:26" ht="21.3" customHeight="1">
-      <c r="A35" s="97"/>
+      <c r="A35" s="120"/>
       <c r="B35" s="48">
         <f>SQRT(V31*10^6/10^18)*2^96</f>
         <v>4.3829404692999735E+24</v>
@@ -4919,13 +4921,13 @@
         <v>13275.054110200288</v>
       </c>
       <c r="S35" s="56"/>
-      <c r="T35" s="113"/>
-      <c r="U35" s="114"/>
-      <c r="V35" s="114"/>
-      <c r="W35" s="114"/>
-      <c r="X35" s="115"/>
-      <c r="Y35" s="116"/>
-      <c r="Z35" s="117"/>
+      <c r="T35" s="138"/>
+      <c r="U35" s="139"/>
+      <c r="V35" s="139"/>
+      <c r="W35" s="139"/>
+      <c r="X35" s="140"/>
+      <c r="Y35" s="141"/>
+      <c r="Z35" s="142"/>
     </row>
     <row r="36" spans="1:26" ht="21.3" customHeight="1">
       <c r="A36" s="57"/>
@@ -4984,65 +4986,65 @@
       <c r="Z37" s="59"/>
     </row>
     <row r="38" spans="1:26" ht="9.4499999999999993" customHeight="1">
-      <c r="A38" s="98"/>
-      <c r="B38" s="124" t="s">
+      <c r="A38" s="125"/>
+      <c r="B38" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="120"/>
-      <c r="D38" s="120"/>
-      <c r="E38" s="120"/>
-      <c r="F38" s="120"/>
-      <c r="G38" s="120"/>
-      <c r="H38" s="120"/>
-      <c r="I38" s="120"/>
-      <c r="J38" s="120"/>
-      <c r="K38" s="120"/>
-      <c r="L38" s="120"/>
-      <c r="M38" s="120"/>
-      <c r="N38" s="120"/>
-      <c r="O38" s="120"/>
-      <c r="P38" s="120"/>
-      <c r="Q38" s="120"/>
-      <c r="R38" s="120"/>
-      <c r="S38" s="120"/>
-      <c r="T38" s="120"/>
-      <c r="U38" s="120"/>
-      <c r="V38" s="120"/>
-      <c r="W38" s="120"/>
-      <c r="X38" s="120"/>
-      <c r="Y38" s="125"/>
-      <c r="Z38" s="126"/>
+      <c r="C38" s="111"/>
+      <c r="D38" s="111"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="111"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="111"/>
+      <c r="I38" s="111"/>
+      <c r="J38" s="111"/>
+      <c r="K38" s="111"/>
+      <c r="L38" s="111"/>
+      <c r="M38" s="111"/>
+      <c r="N38" s="111"/>
+      <c r="O38" s="111"/>
+      <c r="P38" s="111"/>
+      <c r="Q38" s="111"/>
+      <c r="R38" s="111"/>
+      <c r="S38" s="111"/>
+      <c r="T38" s="111"/>
+      <c r="U38" s="111"/>
+      <c r="V38" s="111"/>
+      <c r="W38" s="111"/>
+      <c r="X38" s="111"/>
+      <c r="Y38" s="128"/>
+      <c r="Z38" s="129"/>
     </row>
     <row r="39" spans="1:26" ht="21.9" customHeight="1">
-      <c r="A39" s="99"/>
-      <c r="B39" s="103"/>
-      <c r="C39" s="103"/>
-      <c r="D39" s="103"/>
-      <c r="E39" s="111"/>
-      <c r="F39" s="111"/>
-      <c r="G39" s="111"/>
-      <c r="H39" s="111"/>
-      <c r="I39" s="111"/>
-      <c r="J39" s="111"/>
-      <c r="K39" s="111"/>
-      <c r="L39" s="111"/>
-      <c r="M39" s="111"/>
-      <c r="N39" s="111"/>
-      <c r="O39" s="111"/>
-      <c r="P39" s="111"/>
-      <c r="Q39" s="111"/>
-      <c r="R39" s="111"/>
-      <c r="S39" s="111"/>
-      <c r="T39" s="111"/>
-      <c r="U39" s="111"/>
-      <c r="V39" s="103"/>
-      <c r="W39" s="103"/>
-      <c r="X39" s="103"/>
-      <c r="Y39" s="120"/>
-      <c r="Z39" s="127"/>
+      <c r="A39" s="126"/>
+      <c r="B39" s="108"/>
+      <c r="C39" s="108"/>
+      <c r="D39" s="108"/>
+      <c r="E39" s="115"/>
+      <c r="F39" s="115"/>
+      <c r="G39" s="115"/>
+      <c r="H39" s="115"/>
+      <c r="I39" s="115"/>
+      <c r="J39" s="115"/>
+      <c r="K39" s="115"/>
+      <c r="L39" s="115"/>
+      <c r="M39" s="115"/>
+      <c r="N39" s="115"/>
+      <c r="O39" s="115"/>
+      <c r="P39" s="115"/>
+      <c r="Q39" s="115"/>
+      <c r="R39" s="115"/>
+      <c r="S39" s="115"/>
+      <c r="T39" s="115"/>
+      <c r="U39" s="115"/>
+      <c r="V39" s="108"/>
+      <c r="W39" s="108"/>
+      <c r="X39" s="108"/>
+      <c r="Y39" s="111"/>
+      <c r="Z39" s="130"/>
     </row>
     <row r="40" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A40" s="100"/>
+      <c r="A40" s="123"/>
       <c r="B40" s="22" t="s">
         <v>4</v>
       </c>
@@ -5054,23 +5056,23 @@
         <f>B42/0.81</f>
         <v>3778.2175195446539</v>
       </c>
-      <c r="E40" s="102"/>
-      <c r="F40" s="103"/>
-      <c r="G40" s="103"/>
-      <c r="H40" s="103"/>
-      <c r="I40" s="103"/>
-      <c r="J40" s="103"/>
-      <c r="K40" s="103"/>
-      <c r="L40" s="103"/>
-      <c r="M40" s="103"/>
-      <c r="N40" s="103"/>
-      <c r="O40" s="103"/>
-      <c r="P40" s="103"/>
-      <c r="Q40" s="103"/>
-      <c r="R40" s="103"/>
-      <c r="S40" s="103"/>
-      <c r="T40" s="103"/>
-      <c r="U40" s="104"/>
+      <c r="E40" s="107"/>
+      <c r="F40" s="108"/>
+      <c r="G40" s="108"/>
+      <c r="H40" s="108"/>
+      <c r="I40" s="108"/>
+      <c r="J40" s="108"/>
+      <c r="K40" s="108"/>
+      <c r="L40" s="108"/>
+      <c r="M40" s="108"/>
+      <c r="N40" s="108"/>
+      <c r="O40" s="108"/>
+      <c r="P40" s="108"/>
+      <c r="Q40" s="108"/>
+      <c r="R40" s="108"/>
+      <c r="S40" s="108"/>
+      <c r="T40" s="108"/>
+      <c r="U40" s="109"/>
       <c r="V40" s="22" t="s">
         <v>4</v>
       </c>
@@ -5086,7 +5088,7 @@
       <c r="Z40" s="119"/>
     </row>
     <row r="41" spans="1:26" ht="23.85" customHeight="1">
-      <c r="A41" s="100"/>
+      <c r="A41" s="123"/>
       <c r="B41" s="25" t="s">
         <v>5</v>
       </c>
@@ -5164,7 +5166,7 @@
       </c>
     </row>
     <row r="42" spans="1:26" ht="40.799999999999997" customHeight="1">
-      <c r="A42" s="101"/>
+      <c r="A42" s="124"/>
       <c r="B42" s="30">
         <f t="shared" si="1"/>
         <v>3060.3561908311699</v>
@@ -5264,7 +5266,7 @@
       </c>
     </row>
     <row r="43" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A43" s="96" t="s">
+      <c r="A43" s="106" t="s">
         <v>28</v>
       </c>
       <c r="B43" s="34" t="s">
@@ -5306,23 +5308,23 @@
       <c r="N43" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O43" s="129" t="s">
+      <c r="O43" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="P43" s="130"/>
-      <c r="Q43" s="130"/>
-      <c r="R43" s="131"/>
-      <c r="S43" s="108"/>
-      <c r="T43" s="105"/>
-      <c r="U43" s="106"/>
-      <c r="V43" s="106"/>
-      <c r="W43" s="106"/>
-      <c r="X43" s="107"/>
-      <c r="Y43" s="108"/>
-      <c r="Z43" s="109"/>
+      <c r="P43" s="104"/>
+      <c r="Q43" s="104"/>
+      <c r="R43" s="105"/>
+      <c r="S43" s="102"/>
+      <c r="T43" s="134"/>
+      <c r="U43" s="116"/>
+      <c r="V43" s="116"/>
+      <c r="W43" s="116"/>
+      <c r="X43" s="135"/>
+      <c r="Y43" s="102"/>
+      <c r="Z43" s="131"/>
     </row>
     <row r="44" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A44" s="96"/>
+      <c r="A44" s="106"/>
       <c r="B44" s="39">
         <f>SQRT(B42*10^6/10^18)*2^96</f>
         <v>4.3829404691790772E+24</v>
@@ -5374,27 +5376,27 @@
         <f>M44-(0.1*E44)*B44</f>
         <v>1.7108169422649108E+43</v>
       </c>
-      <c r="O44" s="128" t="s">
+      <c r="O44" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="P44" s="108"/>
-      <c r="Q44" s="128" t="s">
+      <c r="P44" s="102"/>
+      <c r="Q44" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="R44" s="108"/>
+      <c r="R44" s="102"/>
       <c r="S44" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="T44" s="110"/>
-      <c r="U44" s="111"/>
-      <c r="V44" s="111"/>
-      <c r="W44" s="111"/>
-      <c r="X44" s="112"/>
-      <c r="Y44" s="108"/>
-      <c r="Z44" s="109"/>
+      <c r="T44" s="136"/>
+      <c r="U44" s="115"/>
+      <c r="V44" s="115"/>
+      <c r="W44" s="115"/>
+      <c r="X44" s="137"/>
+      <c r="Y44" s="102"/>
+      <c r="Z44" s="131"/>
     </row>
     <row r="45" spans="1:26" ht="20.85" customHeight="1">
-      <c r="A45" s="96" t="s">
+      <c r="A45" s="106" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="34" t="s">
@@ -5455,16 +5457,16 @@
         <f>(P46-Q45)/2*(1-0.0003)</f>
         <v>-9.6591083419882153</v>
       </c>
-      <c r="T45" s="110"/>
-      <c r="U45" s="111"/>
-      <c r="V45" s="111"/>
-      <c r="W45" s="111"/>
-      <c r="X45" s="112"/>
-      <c r="Y45" s="108"/>
-      <c r="Z45" s="109"/>
+      <c r="T45" s="136"/>
+      <c r="U45" s="115"/>
+      <c r="V45" s="115"/>
+      <c r="W45" s="115"/>
+      <c r="X45" s="137"/>
+      <c r="Y45" s="102"/>
+      <c r="Z45" s="131"/>
     </row>
     <row r="46" spans="1:26" ht="21.3" customHeight="1">
-      <c r="A46" s="97"/>
+      <c r="A46" s="120"/>
       <c r="B46" s="48">
         <f>SQRT(V42*10^6/10^18)*2^96</f>
         <v>4.3829404692999735E+24</v>
@@ -5532,13 +5534,13 @@
         <v>13263.284455341987</v>
       </c>
       <c r="S46" s="56"/>
-      <c r="T46" s="113"/>
-      <c r="U46" s="114"/>
-      <c r="V46" s="114"/>
-      <c r="W46" s="114"/>
-      <c r="X46" s="115"/>
-      <c r="Y46" s="116"/>
-      <c r="Z46" s="117"/>
+      <c r="T46" s="138"/>
+      <c r="U46" s="139"/>
+      <c r="V46" s="139"/>
+      <c r="W46" s="139"/>
+      <c r="X46" s="140"/>
+      <c r="Y46" s="141"/>
+      <c r="Z46" s="142"/>
     </row>
     <row r="47" spans="1:26" ht="21.3" customHeight="1">
       <c r="A47" s="57"/>
@@ -5597,65 +5599,65 @@
       <c r="Z48" s="59"/>
     </row>
     <row r="49" spans="1:26" ht="9.4499999999999993" customHeight="1">
-      <c r="A49" s="98"/>
-      <c r="B49" s="124" t="s">
+      <c r="A49" s="125"/>
+      <c r="B49" s="127" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="120"/>
-      <c r="D49" s="120"/>
-      <c r="E49" s="120"/>
-      <c r="F49" s="120"/>
-      <c r="G49" s="120"/>
-      <c r="H49" s="120"/>
-      <c r="I49" s="120"/>
-      <c r="J49" s="120"/>
-      <c r="K49" s="120"/>
-      <c r="L49" s="120"/>
-      <c r="M49" s="120"/>
-      <c r="N49" s="120"/>
-      <c r="O49" s="120"/>
-      <c r="P49" s="120"/>
-      <c r="Q49" s="120"/>
-      <c r="R49" s="120"/>
-      <c r="S49" s="120"/>
-      <c r="T49" s="120"/>
-      <c r="U49" s="120"/>
-      <c r="V49" s="120"/>
-      <c r="W49" s="120"/>
-      <c r="X49" s="120"/>
-      <c r="Y49" s="125"/>
-      <c r="Z49" s="126"/>
+      <c r="C49" s="111"/>
+      <c r="D49" s="111"/>
+      <c r="E49" s="111"/>
+      <c r="F49" s="111"/>
+      <c r="G49" s="111"/>
+      <c r="H49" s="111"/>
+      <c r="I49" s="111"/>
+      <c r="J49" s="111"/>
+      <c r="K49" s="111"/>
+      <c r="L49" s="111"/>
+      <c r="M49" s="111"/>
+      <c r="N49" s="111"/>
+      <c r="O49" s="111"/>
+      <c r="P49" s="111"/>
+      <c r="Q49" s="111"/>
+      <c r="R49" s="111"/>
+      <c r="S49" s="111"/>
+      <c r="T49" s="111"/>
+      <c r="U49" s="111"/>
+      <c r="V49" s="111"/>
+      <c r="W49" s="111"/>
+      <c r="X49" s="111"/>
+      <c r="Y49" s="128"/>
+      <c r="Z49" s="129"/>
     </row>
     <row r="50" spans="1:26" ht="21.9" customHeight="1">
-      <c r="A50" s="99"/>
-      <c r="B50" s="103"/>
-      <c r="C50" s="103"/>
-      <c r="D50" s="103"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="111"/>
-      <c r="J50" s="111"/>
-      <c r="K50" s="111"/>
-      <c r="L50" s="111"/>
-      <c r="M50" s="111"/>
-      <c r="N50" s="111"/>
-      <c r="O50" s="111"/>
-      <c r="P50" s="111"/>
-      <c r="Q50" s="111"/>
-      <c r="R50" s="111"/>
-      <c r="S50" s="111"/>
-      <c r="T50" s="111"/>
-      <c r="U50" s="111"/>
-      <c r="V50" s="103"/>
-      <c r="W50" s="103"/>
-      <c r="X50" s="103"/>
-      <c r="Y50" s="120"/>
-      <c r="Z50" s="127"/>
+      <c r="A50" s="126"/>
+      <c r="B50" s="108"/>
+      <c r="C50" s="108"/>
+      <c r="D50" s="108"/>
+      <c r="E50" s="115"/>
+      <c r="F50" s="115"/>
+      <c r="G50" s="115"/>
+      <c r="H50" s="115"/>
+      <c r="I50" s="115"/>
+      <c r="J50" s="115"/>
+      <c r="K50" s="115"/>
+      <c r="L50" s="115"/>
+      <c r="M50" s="115"/>
+      <c r="N50" s="115"/>
+      <c r="O50" s="115"/>
+      <c r="P50" s="115"/>
+      <c r="Q50" s="115"/>
+      <c r="R50" s="115"/>
+      <c r="S50" s="115"/>
+      <c r="T50" s="115"/>
+      <c r="U50" s="115"/>
+      <c r="V50" s="108"/>
+      <c r="W50" s="108"/>
+      <c r="X50" s="108"/>
+      <c r="Y50" s="111"/>
+      <c r="Z50" s="130"/>
     </row>
     <row r="51" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A51" s="100"/>
+      <c r="A51" s="123"/>
       <c r="B51" s="22" t="s">
         <v>4</v>
       </c>
@@ -5667,23 +5669,23 @@
         <f>B53/0.81</f>
         <v>3778.2175195446539</v>
       </c>
-      <c r="E51" s="102"/>
-      <c r="F51" s="103"/>
-      <c r="G51" s="103"/>
-      <c r="H51" s="103"/>
-      <c r="I51" s="103"/>
-      <c r="J51" s="103"/>
-      <c r="K51" s="103"/>
-      <c r="L51" s="103"/>
-      <c r="M51" s="103"/>
-      <c r="N51" s="103"/>
-      <c r="O51" s="103"/>
-      <c r="P51" s="103"/>
-      <c r="Q51" s="103"/>
-      <c r="R51" s="103"/>
-      <c r="S51" s="103"/>
-      <c r="T51" s="103"/>
-      <c r="U51" s="104"/>
+      <c r="E51" s="107"/>
+      <c r="F51" s="108"/>
+      <c r="G51" s="108"/>
+      <c r="H51" s="108"/>
+      <c r="I51" s="108"/>
+      <c r="J51" s="108"/>
+      <c r="K51" s="108"/>
+      <c r="L51" s="108"/>
+      <c r="M51" s="108"/>
+      <c r="N51" s="108"/>
+      <c r="O51" s="108"/>
+      <c r="P51" s="108"/>
+      <c r="Q51" s="108"/>
+      <c r="R51" s="108"/>
+      <c r="S51" s="108"/>
+      <c r="T51" s="108"/>
+      <c r="U51" s="109"/>
       <c r="V51" s="22" t="s">
         <v>4</v>
       </c>
@@ -5699,7 +5701,7 @@
       <c r="Z51" s="119"/>
     </row>
     <row r="52" spans="1:26" ht="23.85" customHeight="1">
-      <c r="A52" s="100"/>
+      <c r="A52" s="123"/>
       <c r="B52" s="25" t="s">
         <v>5</v>
       </c>
@@ -5777,7 +5779,7 @@
       </c>
     </row>
     <row r="53" spans="1:26" ht="40.65" customHeight="1">
-      <c r="A53" s="101"/>
+      <c r="A53" s="124"/>
       <c r="B53" s="30">
         <f t="shared" si="1"/>
         <v>3060.3561908311699</v>
@@ -5878,7 +5880,7 @@
       </c>
     </row>
     <row r="54" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A54" s="96" t="s">
+      <c r="A54" s="106" t="s">
         <v>28</v>
       </c>
       <c r="B54" s="34" t="s">
@@ -5920,23 +5922,23 @@
       <c r="N54" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O54" s="129" t="s">
+      <c r="O54" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="P54" s="130"/>
-      <c r="Q54" s="130"/>
-      <c r="R54" s="131"/>
-      <c r="S54" s="108"/>
-      <c r="T54" s="105"/>
-      <c r="U54" s="106"/>
-      <c r="V54" s="106"/>
-      <c r="W54" s="106"/>
-      <c r="X54" s="107"/>
-      <c r="Y54" s="108"/>
-      <c r="Z54" s="109"/>
+      <c r="P54" s="104"/>
+      <c r="Q54" s="104"/>
+      <c r="R54" s="105"/>
+      <c r="S54" s="102"/>
+      <c r="T54" s="134"/>
+      <c r="U54" s="116"/>
+      <c r="V54" s="116"/>
+      <c r="W54" s="116"/>
+      <c r="X54" s="135"/>
+      <c r="Y54" s="102"/>
+      <c r="Z54" s="131"/>
     </row>
     <row r="55" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A55" s="96"/>
+      <c r="A55" s="106"/>
       <c r="B55" s="39">
         <f>SQRT(B53*10^6/10^18)*2^96</f>
         <v>4.3829404691790772E+24</v>
@@ -5988,27 +5990,27 @@
         <f>M55-(0.1*E55)*B55</f>
         <v>1.2889378916075946E+43</v>
       </c>
-      <c r="O55" s="128" t="s">
+      <c r="O55" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="P55" s="108"/>
-      <c r="Q55" s="128" t="s">
+      <c r="P55" s="102"/>
+      <c r="Q55" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="R55" s="108"/>
+      <c r="R55" s="102"/>
       <c r="S55" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="T55" s="110"/>
-      <c r="U55" s="111"/>
-      <c r="V55" s="111"/>
-      <c r="W55" s="111"/>
-      <c r="X55" s="112"/>
-      <c r="Y55" s="108"/>
-      <c r="Z55" s="109"/>
+      <c r="T55" s="136"/>
+      <c r="U55" s="115"/>
+      <c r="V55" s="115"/>
+      <c r="W55" s="115"/>
+      <c r="X55" s="137"/>
+      <c r="Y55" s="102"/>
+      <c r="Z55" s="131"/>
     </row>
     <row r="56" spans="1:26" ht="32.85" customHeight="1">
-      <c r="A56" s="96" t="s">
+      <c r="A56" s="106" t="s">
         <v>46</v>
       </c>
       <c r="B56" s="34" t="s">
@@ -6069,16 +6071,16 @@
         <f>(P57-Q56)/2*(1-0.0003)</f>
         <v>3265.8246085298442</v>
       </c>
-      <c r="T56" s="110"/>
-      <c r="U56" s="111"/>
-      <c r="V56" s="111"/>
-      <c r="W56" s="111"/>
-      <c r="X56" s="112"/>
-      <c r="Y56" s="108"/>
-      <c r="Z56" s="109"/>
+      <c r="T56" s="136"/>
+      <c r="U56" s="115"/>
+      <c r="V56" s="115"/>
+      <c r="W56" s="115"/>
+      <c r="X56" s="137"/>
+      <c r="Y56" s="102"/>
+      <c r="Z56" s="131"/>
     </row>
     <row r="57" spans="1:26" ht="21.3" customHeight="1">
-      <c r="A57" s="97"/>
+      <c r="A57" s="120"/>
       <c r="B57" s="48">
         <f>SQRT(V53*10^6/10^18)*2^96</f>
         <v>3.1336255121447264E+24</v>
@@ -6146,13 +6148,13 @@
         <v>7861.8693714701558</v>
       </c>
       <c r="S57" s="56"/>
-      <c r="T57" s="113"/>
-      <c r="U57" s="114"/>
-      <c r="V57" s="114"/>
-      <c r="W57" s="114"/>
-      <c r="X57" s="115"/>
-      <c r="Y57" s="116"/>
-      <c r="Z57" s="117"/>
+      <c r="T57" s="138"/>
+      <c r="U57" s="139"/>
+      <c r="V57" s="139"/>
+      <c r="W57" s="139"/>
+      <c r="X57" s="140"/>
+      <c r="Y57" s="141"/>
+      <c r="Z57" s="142"/>
     </row>
     <row r="58" spans="1:26" ht="21.3" customHeight="1">
       <c r="A58" s="57"/>
@@ -6211,65 +6213,65 @@
       <c r="Z59" s="67"/>
     </row>
     <row r="60" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A60" s="98"/>
+      <c r="A60" s="125"/>
       <c r="B60" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="106"/>
-      <c r="D60" s="106"/>
-      <c r="E60" s="106"/>
-      <c r="F60" s="106"/>
-      <c r="G60" s="106"/>
-      <c r="H60" s="106"/>
-      <c r="I60" s="106"/>
-      <c r="J60" s="106"/>
-      <c r="K60" s="106"/>
-      <c r="L60" s="106"/>
-      <c r="M60" s="106"/>
-      <c r="N60" s="106"/>
-      <c r="O60" s="106"/>
-      <c r="P60" s="106"/>
-      <c r="Q60" s="106"/>
-      <c r="R60" s="106"/>
-      <c r="S60" s="106"/>
-      <c r="T60" s="106"/>
-      <c r="U60" s="106"/>
-      <c r="V60" s="106"/>
-      <c r="W60" s="106"/>
-      <c r="X60" s="106"/>
-      <c r="Y60" s="130"/>
+      <c r="C60" s="116"/>
+      <c r="D60" s="116"/>
+      <c r="E60" s="116"/>
+      <c r="F60" s="116"/>
+      <c r="G60" s="116"/>
+      <c r="H60" s="116"/>
+      <c r="I60" s="116"/>
+      <c r="J60" s="116"/>
+      <c r="K60" s="116"/>
+      <c r="L60" s="116"/>
+      <c r="M60" s="116"/>
+      <c r="N60" s="116"/>
+      <c r="O60" s="116"/>
+      <c r="P60" s="116"/>
+      <c r="Q60" s="116"/>
+      <c r="R60" s="116"/>
+      <c r="S60" s="116"/>
+      <c r="T60" s="116"/>
+      <c r="U60" s="116"/>
+      <c r="V60" s="116"/>
+      <c r="W60" s="116"/>
+      <c r="X60" s="116"/>
+      <c r="Y60" s="104"/>
       <c r="Z60" s="133"/>
     </row>
     <row r="61" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A61" s="99"/>
-      <c r="B61" s="103"/>
-      <c r="C61" s="103"/>
-      <c r="D61" s="103"/>
-      <c r="E61" s="111"/>
-      <c r="F61" s="111"/>
-      <c r="G61" s="111"/>
-      <c r="H61" s="111"/>
-      <c r="I61" s="111"/>
-      <c r="J61" s="111"/>
-      <c r="K61" s="111"/>
-      <c r="L61" s="111"/>
-      <c r="M61" s="111"/>
-      <c r="N61" s="111"/>
-      <c r="O61" s="111"/>
-      <c r="P61" s="111"/>
-      <c r="Q61" s="111"/>
-      <c r="R61" s="111"/>
-      <c r="S61" s="111"/>
-      <c r="T61" s="111"/>
-      <c r="U61" s="111"/>
-      <c r="V61" s="103"/>
-      <c r="W61" s="103"/>
-      <c r="X61" s="103"/>
-      <c r="Y61" s="106"/>
-      <c r="Z61" s="134"/>
+      <c r="A61" s="126"/>
+      <c r="B61" s="108"/>
+      <c r="C61" s="108"/>
+      <c r="D61" s="108"/>
+      <c r="E61" s="115"/>
+      <c r="F61" s="115"/>
+      <c r="G61" s="115"/>
+      <c r="H61" s="115"/>
+      <c r="I61" s="115"/>
+      <c r="J61" s="115"/>
+      <c r="K61" s="115"/>
+      <c r="L61" s="115"/>
+      <c r="M61" s="115"/>
+      <c r="N61" s="115"/>
+      <c r="O61" s="115"/>
+      <c r="P61" s="115"/>
+      <c r="Q61" s="115"/>
+      <c r="R61" s="115"/>
+      <c r="S61" s="115"/>
+      <c r="T61" s="115"/>
+      <c r="U61" s="115"/>
+      <c r="V61" s="108"/>
+      <c r="W61" s="108"/>
+      <c r="X61" s="108"/>
+      <c r="Y61" s="116"/>
+      <c r="Z61" s="117"/>
     </row>
     <row r="62" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A62" s="100"/>
+      <c r="A62" s="123"/>
       <c r="B62" s="22" t="s">
         <v>4</v>
       </c>
@@ -6281,23 +6283,23 @@
         <f>B64/0.81</f>
         <v>3778.1061728382715</v>
       </c>
-      <c r="E62" s="102"/>
-      <c r="F62" s="103"/>
-      <c r="G62" s="103"/>
-      <c r="H62" s="103"/>
-      <c r="I62" s="103"/>
-      <c r="J62" s="103"/>
-      <c r="K62" s="103"/>
-      <c r="L62" s="103"/>
-      <c r="M62" s="103"/>
-      <c r="N62" s="103"/>
-      <c r="O62" s="103"/>
-      <c r="P62" s="103"/>
-      <c r="Q62" s="103"/>
-      <c r="R62" s="103"/>
-      <c r="S62" s="103"/>
-      <c r="T62" s="103"/>
-      <c r="U62" s="104"/>
+      <c r="E62" s="107"/>
+      <c r="F62" s="108"/>
+      <c r="G62" s="108"/>
+      <c r="H62" s="108"/>
+      <c r="I62" s="108"/>
+      <c r="J62" s="108"/>
+      <c r="K62" s="108"/>
+      <c r="L62" s="108"/>
+      <c r="M62" s="108"/>
+      <c r="N62" s="108"/>
+      <c r="O62" s="108"/>
+      <c r="P62" s="108"/>
+      <c r="Q62" s="108"/>
+      <c r="R62" s="108"/>
+      <c r="S62" s="108"/>
+      <c r="T62" s="108"/>
+      <c r="U62" s="109"/>
       <c r="V62" s="22" t="s">
         <v>4</v>
       </c>
@@ -6313,7 +6315,7 @@
       <c r="Z62" s="119"/>
     </row>
     <row r="63" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A63" s="100"/>
+      <c r="A63" s="123"/>
       <c r="B63" s="68" t="s">
         <v>5</v>
       </c>
@@ -6391,7 +6393,7 @@
       </c>
     </row>
     <row r="64" spans="1:26" ht="36" customHeight="1">
-      <c r="A64" s="101"/>
+      <c r="A64" s="124"/>
       <c r="B64" s="69">
         <f t="shared" ref="B64:D70" si="3">3060.265999999</f>
         <v>3060.2659999990001</v>
@@ -6490,7 +6492,7 @@
       </c>
     </row>
     <row r="65" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A65" s="96" t="s">
+      <c r="A65" s="106" t="s">
         <v>28</v>
       </c>
       <c r="B65" s="34" t="s">
@@ -6532,23 +6534,23 @@
       <c r="N65" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O65" s="129" t="s">
+      <c r="O65" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="P65" s="130"/>
-      <c r="Q65" s="130"/>
-      <c r="R65" s="131"/>
-      <c r="S65" s="109"/>
-      <c r="T65" s="98"/>
-      <c r="U65" s="120"/>
-      <c r="V65" s="120"/>
-      <c r="W65" s="106"/>
-      <c r="X65" s="107"/>
-      <c r="Y65" s="121"/>
-      <c r="Z65" s="122"/>
+      <c r="P65" s="104"/>
+      <c r="Q65" s="104"/>
+      <c r="R65" s="105"/>
+      <c r="S65" s="131"/>
+      <c r="T65" s="125"/>
+      <c r="U65" s="111"/>
+      <c r="V65" s="111"/>
+      <c r="W65" s="116"/>
+      <c r="X65" s="135"/>
+      <c r="Y65" s="143"/>
+      <c r="Z65" s="144"/>
     </row>
     <row r="66" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A66" s="96"/>
+      <c r="A66" s="106"/>
       <c r="B66" s="39">
         <f>SQRT(B64*10^6/10^18)*2^96</f>
         <v>4.382875884546422E+24</v>
@@ -6600,27 +6602,27 @@
         <f>M66-($B$3*E66)*B66</f>
         <v>1.2889611060943387E+43</v>
       </c>
-      <c r="O66" s="128" t="s">
+      <c r="O66" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="P66" s="108"/>
-      <c r="Q66" s="128" t="s">
+      <c r="P66" s="102"/>
+      <c r="Q66" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="R66" s="108"/>
+      <c r="R66" s="102"/>
       <c r="S66" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="T66" s="99"/>
-      <c r="U66" s="111"/>
-      <c r="V66" s="111"/>
-      <c r="W66" s="111"/>
-      <c r="X66" s="112"/>
-      <c r="Y66" s="108"/>
-      <c r="Z66" s="109"/>
+      <c r="T66" s="126"/>
+      <c r="U66" s="115"/>
+      <c r="V66" s="115"/>
+      <c r="W66" s="115"/>
+      <c r="X66" s="137"/>
+      <c r="Y66" s="102"/>
+      <c r="Z66" s="131"/>
     </row>
     <row r="67" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A67" s="96" t="s">
+      <c r="A67" s="106" t="s">
         <v>46</v>
       </c>
       <c r="B67" s="34" t="s">
@@ -6681,16 +6683,16 @@
         <f>(P68-Q67)/2*(1-0.0003)</f>
         <v>-0.42613968412199249</v>
       </c>
-      <c r="T67" s="99"/>
-      <c r="U67" s="111"/>
-      <c r="V67" s="111"/>
-      <c r="W67" s="111"/>
-      <c r="X67" s="112"/>
-      <c r="Y67" s="108"/>
-      <c r="Z67" s="109"/>
+      <c r="T67" s="126"/>
+      <c r="U67" s="115"/>
+      <c r="V67" s="115"/>
+      <c r="W67" s="115"/>
+      <c r="X67" s="137"/>
+      <c r="Y67" s="102"/>
+      <c r="Z67" s="131"/>
     </row>
     <row r="68" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A68" s="97"/>
+      <c r="A68" s="120"/>
       <c r="B68" s="48">
         <f>SQRT(V64*10^6/10^18)*2^96</f>
         <v>4.3829404692999735E+24</v>
@@ -6758,13 +6760,13 @@
         <v>10000.426139684121</v>
       </c>
       <c r="S68" s="75"/>
-      <c r="T68" s="123"/>
-      <c r="U68" s="114"/>
-      <c r="V68" s="114"/>
-      <c r="W68" s="114"/>
-      <c r="X68" s="115"/>
-      <c r="Y68" s="116"/>
-      <c r="Z68" s="117"/>
+      <c r="T68" s="145"/>
+      <c r="U68" s="139"/>
+      <c r="V68" s="139"/>
+      <c r="W68" s="139"/>
+      <c r="X68" s="140"/>
+      <c r="Y68" s="141"/>
+      <c r="Z68" s="142"/>
     </row>
     <row r="69" spans="1:26" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="76"/>
@@ -7116,28 +7118,29 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A1:X1"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="O10:S10"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="E7:U7"/>
-    <mergeCell ref="B5:Z6"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="E62:U62"/>
+    <mergeCell ref="T10:Z13"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="Y29:Z29"/>
+    <mergeCell ref="Y40:Z40"/>
+    <mergeCell ref="Y51:Z51"/>
+    <mergeCell ref="Y62:Z62"/>
+    <mergeCell ref="T21:Z24"/>
+    <mergeCell ref="T32:Z35"/>
+    <mergeCell ref="T43:Z46"/>
+    <mergeCell ref="T54:Z57"/>
+    <mergeCell ref="T65:Z68"/>
+    <mergeCell ref="B16:Z17"/>
+    <mergeCell ref="O55:P55"/>
+    <mergeCell ref="Q55:R55"/>
+    <mergeCell ref="O54:S54"/>
+    <mergeCell ref="O66:P66"/>
+    <mergeCell ref="Q66:R66"/>
+    <mergeCell ref="O65:S65"/>
+    <mergeCell ref="B60:Z61"/>
     <mergeCell ref="E18:U18"/>
     <mergeCell ref="E29:U29"/>
     <mergeCell ref="E40:U40"/>
@@ -7154,29 +7157,28 @@
     <mergeCell ref="B27:Z28"/>
     <mergeCell ref="B38:Z39"/>
     <mergeCell ref="B49:Z50"/>
-    <mergeCell ref="O55:P55"/>
-    <mergeCell ref="Q55:R55"/>
-    <mergeCell ref="O54:S54"/>
-    <mergeCell ref="O66:P66"/>
-    <mergeCell ref="Q66:R66"/>
-    <mergeCell ref="O65:S65"/>
-    <mergeCell ref="B60:Z61"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="E62:U62"/>
-    <mergeCell ref="T10:Z13"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="Y40:Z40"/>
-    <mergeCell ref="Y51:Z51"/>
-    <mergeCell ref="Y62:Z62"/>
-    <mergeCell ref="T21:Z24"/>
-    <mergeCell ref="T32:Z35"/>
-    <mergeCell ref="T43:Z46"/>
-    <mergeCell ref="T54:Z57"/>
-    <mergeCell ref="T65:Z68"/>
-    <mergeCell ref="B16:Z17"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="O10:S10"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="E7:U7"/>
+    <mergeCell ref="B5:Z6"/>
+    <mergeCell ref="Y7:Z7"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup scale="72" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat : rebal uni scenario, fix: adjustTicks (#26)
* issue : sqrtUp revert

* Fix huge price

* fix: adjustTicks, feat : rebal uni move out scenario

Co-authored-by: LeadDev <leaddev@anon.farm>
</commit_message>
<xml_diff>
--- a/test/scenarios/Rebalance_Test.xlsx
+++ b/test/scenarios/Rebalance_Test.xlsx
@@ -1679,6 +1679,129 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1694,39 +1817,9 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1734,99 +1827,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2991,8 +2991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N7" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -3019,38 +3019,39 @@
     <col min="21" max="21" width="35.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="29" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="31.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="25.21875" style="95" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.21875" style="95" customWidth="1"/>
+    <col min="26" max="26" width="25.21875" style="95" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16.33203125" style="2" customWidth="1"/>
     <col min="28" max="16384" width="16.33203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27.6" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="98"/>
-      <c r="S1" s="98"/>
-      <c r="T1" s="98"/>
-      <c r="U1" s="98"/>
-      <c r="V1" s="98"/>
-      <c r="W1" s="98"/>
-      <c r="X1" s="100"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
+      <c r="L1" s="139"/>
+      <c r="M1" s="139"/>
+      <c r="N1" s="139"/>
+      <c r="O1" s="139"/>
+      <c r="P1" s="139"/>
+      <c r="Q1" s="139"/>
+      <c r="R1" s="139"/>
+      <c r="S1" s="139"/>
+      <c r="T1" s="139"/>
+      <c r="U1" s="139"/>
+      <c r="V1" s="139"/>
+      <c r="W1" s="139"/>
+      <c r="X1" s="141"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
@@ -3148,65 +3149,65 @@
       <c r="Z4" s="21"/>
     </row>
     <row r="5" spans="1:26" ht="9.4499999999999993" customHeight="1">
-      <c r="A5" s="121"/>
-      <c r="B5" s="110" t="s">
+      <c r="A5" s="135"/>
+      <c r="B5" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="111"/>
-      <c r="L5" s="111"/>
-      <c r="M5" s="111"/>
-      <c r="N5" s="111"/>
-      <c r="O5" s="111"/>
-      <c r="P5" s="111"/>
-      <c r="Q5" s="111"/>
-      <c r="R5" s="111"/>
-      <c r="S5" s="111"/>
-      <c r="T5" s="111"/>
-      <c r="U5" s="111"/>
-      <c r="V5" s="111"/>
-      <c r="W5" s="111"/>
-      <c r="X5" s="111"/>
-      <c r="Y5" s="112"/>
-      <c r="Z5" s="113"/>
+      <c r="C5" s="120"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="120"/>
+      <c r="P5" s="120"/>
+      <c r="Q5" s="120"/>
+      <c r="R5" s="120"/>
+      <c r="S5" s="120"/>
+      <c r="T5" s="120"/>
+      <c r="U5" s="120"/>
+      <c r="V5" s="120"/>
+      <c r="W5" s="120"/>
+      <c r="X5" s="120"/>
+      <c r="Y5" s="143"/>
+      <c r="Z5" s="144"/>
     </row>
     <row r="6" spans="1:26" ht="21.9" customHeight="1">
-      <c r="A6" s="122"/>
-      <c r="B6" s="114"/>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="115"/>
-      <c r="O6" s="115"/>
-      <c r="P6" s="115"/>
-      <c r="Q6" s="115"/>
-      <c r="R6" s="115"/>
-      <c r="S6" s="115"/>
-      <c r="T6" s="115"/>
-      <c r="U6" s="115"/>
-      <c r="V6" s="108"/>
-      <c r="W6" s="108"/>
-      <c r="X6" s="108"/>
-      <c r="Y6" s="116"/>
-      <c r="Z6" s="117"/>
+      <c r="A6" s="136"/>
+      <c r="B6" s="145"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="111"/>
+      <c r="L6" s="111"/>
+      <c r="M6" s="111"/>
+      <c r="N6" s="111"/>
+      <c r="O6" s="111"/>
+      <c r="P6" s="111"/>
+      <c r="Q6" s="111"/>
+      <c r="R6" s="111"/>
+      <c r="S6" s="111"/>
+      <c r="T6" s="111"/>
+      <c r="U6" s="111"/>
+      <c r="V6" s="103"/>
+      <c r="W6" s="103"/>
+      <c r="X6" s="103"/>
+      <c r="Y6" s="106"/>
+      <c r="Z6" s="134"/>
     </row>
     <row r="7" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A7" s="123"/>
+      <c r="A7" s="100"/>
       <c r="B7" s="22" t="s">
         <v>4</v>
       </c>
@@ -3218,23 +3219,23 @@
         <f>B9/0.81</f>
         <v>3778.2175195446539</v>
       </c>
-      <c r="E7" s="107"/>
-      <c r="F7" s="108"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="108"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="108"/>
-      <c r="O7" s="108"/>
-      <c r="P7" s="108"/>
-      <c r="Q7" s="108"/>
-      <c r="R7" s="108"/>
-      <c r="S7" s="108"/>
-      <c r="T7" s="108"/>
-      <c r="U7" s="109"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="103"/>
+      <c r="R7" s="103"/>
+      <c r="S7" s="103"/>
+      <c r="T7" s="103"/>
+      <c r="U7" s="104"/>
       <c r="V7" s="22" t="s">
         <v>4</v>
       </c>
@@ -3250,7 +3251,7 @@
       <c r="Z7" s="119"/>
     </row>
     <row r="8" spans="1:26" ht="23.85" customHeight="1">
-      <c r="A8" s="123"/>
+      <c r="A8" s="100"/>
       <c r="B8" s="25" t="s">
         <v>5</v>
       </c>
@@ -3328,7 +3329,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="39.9" customHeight="1">
-      <c r="A9" s="124"/>
+      <c r="A9" s="101"/>
       <c r="B9" s="30">
         <f>3060.35619083117</f>
         <v>3060.3561908311699</v>
@@ -3427,7 +3428,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A10" s="106" t="s">
+      <c r="A10" s="96" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="34" t="s">
@@ -3469,23 +3470,23 @@
       <c r="N10" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O10" s="103" t="s">
+      <c r="O10" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="P10" s="104"/>
-      <c r="Q10" s="104"/>
-      <c r="R10" s="105"/>
-      <c r="S10" s="102"/>
-      <c r="T10" s="134"/>
-      <c r="U10" s="116"/>
-      <c r="V10" s="116"/>
-      <c r="W10" s="116"/>
-      <c r="X10" s="135"/>
-      <c r="Y10" s="102"/>
-      <c r="Z10" s="131"/>
+      <c r="P10" s="130"/>
+      <c r="Q10" s="130"/>
+      <c r="R10" s="131"/>
+      <c r="S10" s="108"/>
+      <c r="T10" s="105"/>
+      <c r="U10" s="106"/>
+      <c r="V10" s="106"/>
+      <c r="W10" s="106"/>
+      <c r="X10" s="107"/>
+      <c r="Y10" s="108"/>
+      <c r="Z10" s="109"/>
     </row>
     <row r="11" spans="1:26" ht="27.75" customHeight="1">
-      <c r="A11" s="106"/>
+      <c r="A11" s="96"/>
       <c r="B11" s="39">
         <f>SQRT(B9*10^6/10^18)*2^96</f>
         <v>4.3829404691790772E+24</v>
@@ -3537,27 +3538,27 @@
         <f>M11-($B$3*E11)*B11</f>
         <v>1.2889378916075946E+43</v>
       </c>
-      <c r="O11" s="101" t="s">
+      <c r="O11" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="P11" s="102"/>
-      <c r="Q11" s="101" t="s">
+      <c r="P11" s="108"/>
+      <c r="Q11" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="R11" s="102"/>
+      <c r="R11" s="108"/>
       <c r="S11" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="T11" s="136"/>
-      <c r="U11" s="115"/>
-      <c r="V11" s="115"/>
-      <c r="W11" s="115"/>
-      <c r="X11" s="137"/>
-      <c r="Y11" s="102"/>
-      <c r="Z11" s="131"/>
+      <c r="T11" s="110"/>
+      <c r="U11" s="111"/>
+      <c r="V11" s="111"/>
+      <c r="W11" s="111"/>
+      <c r="X11" s="112"/>
+      <c r="Y11" s="108"/>
+      <c r="Z11" s="109"/>
     </row>
     <row r="12" spans="1:26" ht="20.85" customHeight="1">
-      <c r="A12" s="106" t="s">
+      <c r="A12" s="96" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="34" t="s">
@@ -3618,16 +3619,16 @@
         <f>(P13-Q12)/2*(1-0.0003)</f>
         <v>-0.42613940834773056</v>
       </c>
-      <c r="T12" s="136"/>
-      <c r="U12" s="115"/>
-      <c r="V12" s="115"/>
-      <c r="W12" s="115"/>
-      <c r="X12" s="137"/>
-      <c r="Y12" s="102"/>
-      <c r="Z12" s="131"/>
+      <c r="T12" s="110"/>
+      <c r="U12" s="111"/>
+      <c r="V12" s="111"/>
+      <c r="W12" s="111"/>
+      <c r="X12" s="112"/>
+      <c r="Y12" s="108"/>
+      <c r="Z12" s="109"/>
     </row>
     <row r="13" spans="1:26" ht="30" customHeight="1">
-      <c r="A13" s="120"/>
+      <c r="A13" s="97"/>
       <c r="B13" s="48">
         <f>SQRT(V9*10^6/10^18)*2^96</f>
         <v>4.3972388145443278E+24</v>
@@ -3695,13 +3696,13 @@
         <v>10000.426139408348</v>
       </c>
       <c r="S13" s="56"/>
-      <c r="T13" s="138"/>
-      <c r="U13" s="139"/>
-      <c r="V13" s="139"/>
-      <c r="W13" s="139"/>
-      <c r="X13" s="140"/>
-      <c r="Y13" s="141"/>
-      <c r="Z13" s="142"/>
+      <c r="T13" s="113"/>
+      <c r="U13" s="114"/>
+      <c r="V13" s="114"/>
+      <c r="W13" s="114"/>
+      <c r="X13" s="115"/>
+      <c r="Y13" s="116"/>
+      <c r="Z13" s="117"/>
     </row>
     <row r="14" spans="1:26" ht="21.3" customHeight="1">
       <c r="A14" s="57"/>
@@ -3760,65 +3761,65 @@
       <c r="Z15" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="9.4499999999999993" customHeight="1">
-      <c r="A16" s="125"/>
-      <c r="B16" s="127" t="s">
+      <c r="A16" s="98"/>
+      <c r="B16" s="124" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="111"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="111"/>
-      <c r="H16" s="111"/>
-      <c r="I16" s="111"/>
-      <c r="J16" s="111"/>
-      <c r="K16" s="111"/>
-      <c r="L16" s="111"/>
-      <c r="M16" s="111"/>
-      <c r="N16" s="111"/>
-      <c r="O16" s="111"/>
-      <c r="P16" s="111"/>
-      <c r="Q16" s="111"/>
-      <c r="R16" s="111"/>
-      <c r="S16" s="111"/>
-      <c r="T16" s="111"/>
-      <c r="U16" s="111"/>
-      <c r="V16" s="111"/>
-      <c r="W16" s="111"/>
-      <c r="X16" s="111"/>
-      <c r="Y16" s="128"/>
-      <c r="Z16" s="129"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
+      <c r="F16" s="120"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="120"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="120"/>
+      <c r="N16" s="120"/>
+      <c r="O16" s="120"/>
+      <c r="P16" s="120"/>
+      <c r="Q16" s="120"/>
+      <c r="R16" s="120"/>
+      <c r="S16" s="120"/>
+      <c r="T16" s="120"/>
+      <c r="U16" s="120"/>
+      <c r="V16" s="120"/>
+      <c r="W16" s="120"/>
+      <c r="X16" s="120"/>
+      <c r="Y16" s="125"/>
+      <c r="Z16" s="126"/>
     </row>
     <row r="17" spans="1:26" ht="21.9" customHeight="1">
-      <c r="A17" s="126"/>
-      <c r="B17" s="108"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="115"/>
-      <c r="H17" s="115"/>
-      <c r="I17" s="115"/>
-      <c r="J17" s="115"/>
-      <c r="K17" s="115"/>
-      <c r="L17" s="115"/>
-      <c r="M17" s="115"/>
-      <c r="N17" s="115"/>
-      <c r="O17" s="115"/>
-      <c r="P17" s="115"/>
-      <c r="Q17" s="115"/>
-      <c r="R17" s="115"/>
-      <c r="S17" s="115"/>
-      <c r="T17" s="115"/>
-      <c r="U17" s="115"/>
-      <c r="V17" s="108"/>
-      <c r="W17" s="108"/>
-      <c r="X17" s="108"/>
-      <c r="Y17" s="111"/>
-      <c r="Z17" s="130"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="103"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="111"/>
+      <c r="I17" s="111"/>
+      <c r="J17" s="111"/>
+      <c r="K17" s="111"/>
+      <c r="L17" s="111"/>
+      <c r="M17" s="111"/>
+      <c r="N17" s="111"/>
+      <c r="O17" s="111"/>
+      <c r="P17" s="111"/>
+      <c r="Q17" s="111"/>
+      <c r="R17" s="111"/>
+      <c r="S17" s="111"/>
+      <c r="T17" s="111"/>
+      <c r="U17" s="111"/>
+      <c r="V17" s="103"/>
+      <c r="W17" s="103"/>
+      <c r="X17" s="103"/>
+      <c r="Y17" s="120"/>
+      <c r="Z17" s="127"/>
     </row>
     <row r="18" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A18" s="123"/>
+      <c r="A18" s="100"/>
       <c r="B18" s="22" t="s">
         <v>4</v>
       </c>
@@ -3830,23 +3831,23 @@
         <f>B20/0.81</f>
         <v>3778.2175195446539</v>
       </c>
-      <c r="E18" s="107"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="108"/>
-      <c r="J18" s="108"/>
-      <c r="K18" s="108"/>
-      <c r="L18" s="108"/>
-      <c r="M18" s="108"/>
-      <c r="N18" s="108"/>
-      <c r="O18" s="108"/>
-      <c r="P18" s="108"/>
-      <c r="Q18" s="108"/>
-      <c r="R18" s="108"/>
-      <c r="S18" s="108"/>
-      <c r="T18" s="108"/>
-      <c r="U18" s="109"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="103"/>
+      <c r="I18" s="103"/>
+      <c r="J18" s="103"/>
+      <c r="K18" s="103"/>
+      <c r="L18" s="103"/>
+      <c r="M18" s="103"/>
+      <c r="N18" s="103"/>
+      <c r="O18" s="103"/>
+      <c r="P18" s="103"/>
+      <c r="Q18" s="103"/>
+      <c r="R18" s="103"/>
+      <c r="S18" s="103"/>
+      <c r="T18" s="103"/>
+      <c r="U18" s="104"/>
       <c r="V18" s="22" t="s">
         <v>4</v>
       </c>
@@ -3862,7 +3863,7 @@
       <c r="Z18" s="119"/>
     </row>
     <row r="19" spans="1:26" ht="23.85" customHeight="1">
-      <c r="A19" s="123"/>
+      <c r="A19" s="100"/>
       <c r="B19" s="25" t="s">
         <v>5</v>
       </c>
@@ -3940,7 +3941,7 @@
       </c>
     </row>
     <row r="20" spans="1:26" ht="40.5" customHeight="1">
-      <c r="A20" s="124"/>
+      <c r="A20" s="101"/>
       <c r="B20" s="30">
         <f t="shared" ref="B20:B53" si="1">3060.35619083117</f>
         <v>3060.3561908311699</v>
@@ -4040,7 +4041,7 @@
       </c>
     </row>
     <row r="21" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A21" s="106" t="s">
+      <c r="A21" s="96" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="34" t="s">
@@ -4082,23 +4083,23 @@
       <c r="N21" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O21" s="103" t="s">
+      <c r="O21" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="P21" s="104"/>
-      <c r="Q21" s="104"/>
-      <c r="R21" s="105"/>
-      <c r="S21" s="102"/>
-      <c r="T21" s="134"/>
-      <c r="U21" s="116"/>
-      <c r="V21" s="116"/>
-      <c r="W21" s="116"/>
-      <c r="X21" s="135"/>
-      <c r="Y21" s="102"/>
-      <c r="Z21" s="131"/>
+      <c r="P21" s="130"/>
+      <c r="Q21" s="130"/>
+      <c r="R21" s="131"/>
+      <c r="S21" s="108"/>
+      <c r="T21" s="105"/>
+      <c r="U21" s="106"/>
+      <c r="V21" s="106"/>
+      <c r="W21" s="106"/>
+      <c r="X21" s="107"/>
+      <c r="Y21" s="108"/>
+      <c r="Z21" s="109"/>
     </row>
     <row r="22" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A22" s="106"/>
+      <c r="A22" s="96"/>
       <c r="B22" s="39">
         <f>SQRT(B20*10^6/10^18)*2^96</f>
         <v>4.3829404691790772E+24</v>
@@ -4112,7 +4113,7 @@
         <v>4.8699799860470599E+24</v>
       </c>
       <c r="E22" s="41">
-        <f t="shared" si="0"/>
+        <f>3267872074675370000</f>
         <v>3.26787207467537E+18</v>
       </c>
       <c r="F22" s="41">
@@ -4150,27 +4151,27 @@
         <f>M22-(0.1*E22)*B22</f>
         <v>1.2889378916075946E+43</v>
       </c>
-      <c r="O22" s="101" t="s">
+      <c r="O22" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="P22" s="102"/>
-      <c r="Q22" s="101" t="s">
+      <c r="P22" s="108"/>
+      <c r="Q22" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="R22" s="102"/>
+      <c r="R22" s="108"/>
       <c r="S22" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="T22" s="136"/>
-      <c r="U22" s="115"/>
-      <c r="V22" s="115"/>
-      <c r="W22" s="115"/>
-      <c r="X22" s="137"/>
-      <c r="Y22" s="102"/>
-      <c r="Z22" s="131"/>
+      <c r="T22" s="110"/>
+      <c r="U22" s="111"/>
+      <c r="V22" s="111"/>
+      <c r="W22" s="111"/>
+      <c r="X22" s="112"/>
+      <c r="Y22" s="108"/>
+      <c r="Z22" s="109"/>
     </row>
     <row r="23" spans="1:26" ht="20.85" customHeight="1">
-      <c r="A23" s="106" t="s">
+      <c r="A23" s="96" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="34" t="s">
@@ -4231,16 +4232,16 @@
         <f>(P24-Q23)/2*(1-0.0003)</f>
         <v>2554.9234823787783</v>
       </c>
-      <c r="T23" s="136"/>
-      <c r="U23" s="115"/>
-      <c r="V23" s="115"/>
-      <c r="W23" s="115"/>
-      <c r="X23" s="137"/>
-      <c r="Y23" s="102"/>
-      <c r="Z23" s="131"/>
+      <c r="T23" s="110"/>
+      <c r="U23" s="111"/>
+      <c r="V23" s="111"/>
+      <c r="W23" s="111"/>
+      <c r="X23" s="112"/>
+      <c r="Y23" s="108"/>
+      <c r="Z23" s="109"/>
     </row>
     <row r="24" spans="1:26" ht="21.3" customHeight="1">
-      <c r="A24" s="120"/>
+      <c r="A24" s="97"/>
       <c r="B24" s="48">
         <f>SQRT(V20*10^6/10^18)*2^96</f>
         <v>4.3829404692999735E+24</v>
@@ -4308,13 +4309,13 @@
         <v>12557.309431621223</v>
       </c>
       <c r="S24" s="56"/>
-      <c r="T24" s="138"/>
-      <c r="U24" s="139"/>
-      <c r="V24" s="139"/>
-      <c r="W24" s="139"/>
-      <c r="X24" s="140"/>
-      <c r="Y24" s="141"/>
-      <c r="Z24" s="142"/>
+      <c r="T24" s="113"/>
+      <c r="U24" s="114"/>
+      <c r="V24" s="114"/>
+      <c r="W24" s="114"/>
+      <c r="X24" s="115"/>
+      <c r="Y24" s="116"/>
+      <c r="Z24" s="117"/>
     </row>
     <row r="25" spans="1:26" ht="21.3" customHeight="1">
       <c r="A25" s="57"/>
@@ -4373,65 +4374,65 @@
       <c r="Z26" s="59"/>
     </row>
     <row r="27" spans="1:26" ht="9.4499999999999993" customHeight="1">
-      <c r="A27" s="125"/>
-      <c r="B27" s="127" t="s">
+      <c r="A27" s="98"/>
+      <c r="B27" s="124" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="111"/>
-      <c r="H27" s="111"/>
-      <c r="I27" s="111"/>
-      <c r="J27" s="111"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="111"/>
-      <c r="M27" s="111"/>
-      <c r="N27" s="111"/>
-      <c r="O27" s="111"/>
-      <c r="P27" s="111"/>
-      <c r="Q27" s="111"/>
-      <c r="R27" s="111"/>
-      <c r="S27" s="111"/>
-      <c r="T27" s="111"/>
-      <c r="U27" s="111"/>
-      <c r="V27" s="111"/>
-      <c r="W27" s="111"/>
-      <c r="X27" s="111"/>
-      <c r="Y27" s="128"/>
-      <c r="Z27" s="129"/>
+      <c r="C27" s="120"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="120"/>
+      <c r="G27" s="120"/>
+      <c r="H27" s="120"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="120"/>
+      <c r="L27" s="120"/>
+      <c r="M27" s="120"/>
+      <c r="N27" s="120"/>
+      <c r="O27" s="120"/>
+      <c r="P27" s="120"/>
+      <c r="Q27" s="120"/>
+      <c r="R27" s="120"/>
+      <c r="S27" s="120"/>
+      <c r="T27" s="120"/>
+      <c r="U27" s="120"/>
+      <c r="V27" s="120"/>
+      <c r="W27" s="120"/>
+      <c r="X27" s="120"/>
+      <c r="Y27" s="125"/>
+      <c r="Z27" s="126"/>
     </row>
     <row r="28" spans="1:26" ht="21.9" customHeight="1">
-      <c r="A28" s="126"/>
-      <c r="B28" s="108"/>
-      <c r="C28" s="108"/>
-      <c r="D28" s="108"/>
-      <c r="E28" s="115"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="115"/>
-      <c r="H28" s="115"/>
-      <c r="I28" s="115"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="115"/>
-      <c r="L28" s="115"/>
-      <c r="M28" s="115"/>
-      <c r="N28" s="115"/>
-      <c r="O28" s="115"/>
-      <c r="P28" s="115"/>
-      <c r="Q28" s="115"/>
-      <c r="R28" s="115"/>
-      <c r="S28" s="115"/>
-      <c r="T28" s="115"/>
-      <c r="U28" s="115"/>
-      <c r="V28" s="108"/>
-      <c r="W28" s="108"/>
-      <c r="X28" s="108"/>
-      <c r="Y28" s="111"/>
-      <c r="Z28" s="130"/>
+      <c r="A28" s="99"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="111"/>
+      <c r="G28" s="111"/>
+      <c r="H28" s="111"/>
+      <c r="I28" s="111"/>
+      <c r="J28" s="111"/>
+      <c r="K28" s="111"/>
+      <c r="L28" s="111"/>
+      <c r="M28" s="111"/>
+      <c r="N28" s="111"/>
+      <c r="O28" s="111"/>
+      <c r="P28" s="111"/>
+      <c r="Q28" s="111"/>
+      <c r="R28" s="111"/>
+      <c r="S28" s="111"/>
+      <c r="T28" s="111"/>
+      <c r="U28" s="111"/>
+      <c r="V28" s="103"/>
+      <c r="W28" s="103"/>
+      <c r="X28" s="103"/>
+      <c r="Y28" s="120"/>
+      <c r="Z28" s="127"/>
     </row>
     <row r="29" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A29" s="123"/>
+      <c r="A29" s="100"/>
       <c r="B29" s="22" t="s">
         <v>4</v>
       </c>
@@ -4443,23 +4444,23 @@
         <f>B31/0.81</f>
         <v>3778.2175195446539</v>
       </c>
-      <c r="E29" s="107"/>
-      <c r="F29" s="108"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="108"/>
-      <c r="J29" s="108"/>
-      <c r="K29" s="108"/>
-      <c r="L29" s="108"/>
-      <c r="M29" s="108"/>
-      <c r="N29" s="108"/>
-      <c r="O29" s="108"/>
-      <c r="P29" s="108"/>
-      <c r="Q29" s="108"/>
-      <c r="R29" s="108"/>
-      <c r="S29" s="108"/>
-      <c r="T29" s="108"/>
-      <c r="U29" s="109"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="103"/>
+      <c r="J29" s="103"/>
+      <c r="K29" s="103"/>
+      <c r="L29" s="103"/>
+      <c r="M29" s="103"/>
+      <c r="N29" s="103"/>
+      <c r="O29" s="103"/>
+      <c r="P29" s="103"/>
+      <c r="Q29" s="103"/>
+      <c r="R29" s="103"/>
+      <c r="S29" s="103"/>
+      <c r="T29" s="103"/>
+      <c r="U29" s="104"/>
       <c r="V29" s="22" t="s">
         <v>4</v>
       </c>
@@ -4475,7 +4476,7 @@
       <c r="Z29" s="119"/>
     </row>
     <row r="30" spans="1:26" ht="23.85" customHeight="1">
-      <c r="A30" s="123"/>
+      <c r="A30" s="100"/>
       <c r="B30" s="25" t="s">
         <v>5</v>
       </c>
@@ -4553,7 +4554,7 @@
       </c>
     </row>
     <row r="31" spans="1:26" ht="40.35" customHeight="1">
-      <c r="A31" s="124"/>
+      <c r="A31" s="101"/>
       <c r="B31" s="30">
         <f t="shared" si="1"/>
         <v>3060.3561908311699</v>
@@ -4653,7 +4654,7 @@
       </c>
     </row>
     <row r="32" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A32" s="106" t="s">
+      <c r="A32" s="96" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="34" t="s">
@@ -4695,23 +4696,23 @@
       <c r="N32" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O32" s="103" t="s">
+      <c r="O32" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="P32" s="104"/>
-      <c r="Q32" s="104"/>
-      <c r="R32" s="105"/>
-      <c r="S32" s="102"/>
-      <c r="T32" s="134"/>
-      <c r="U32" s="116"/>
-      <c r="V32" s="116"/>
-      <c r="W32" s="116"/>
-      <c r="X32" s="135"/>
-      <c r="Y32" s="102"/>
-      <c r="Z32" s="131"/>
+      <c r="P32" s="130"/>
+      <c r="Q32" s="130"/>
+      <c r="R32" s="131"/>
+      <c r="S32" s="108"/>
+      <c r="T32" s="105"/>
+      <c r="U32" s="106"/>
+      <c r="V32" s="106"/>
+      <c r="W32" s="106"/>
+      <c r="X32" s="107"/>
+      <c r="Y32" s="108"/>
+      <c r="Z32" s="109"/>
     </row>
     <row r="33" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A33" s="106"/>
+      <c r="A33" s="96"/>
       <c r="B33" s="39">
         <f>SQRT(B31*10^6/10^18)*2^96</f>
         <v>4.3829404691790772E+24</v>
@@ -4763,27 +4764,27 @@
         <f>M33-(0.1*E33)*B33</f>
         <v>1.5966769901727963E+43</v>
       </c>
-      <c r="O33" s="101" t="s">
+      <c r="O33" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="P33" s="102"/>
-      <c r="Q33" s="101" t="s">
+      <c r="P33" s="108"/>
+      <c r="Q33" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="R33" s="102"/>
+      <c r="R33" s="108"/>
       <c r="S33" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="T33" s="136"/>
-      <c r="U33" s="115"/>
-      <c r="V33" s="115"/>
-      <c r="W33" s="115"/>
-      <c r="X33" s="137"/>
-      <c r="Y33" s="102"/>
-      <c r="Z33" s="131"/>
+      <c r="T33" s="110"/>
+      <c r="U33" s="111"/>
+      <c r="V33" s="111"/>
+      <c r="W33" s="111"/>
+      <c r="X33" s="112"/>
+      <c r="Y33" s="108"/>
+      <c r="Z33" s="109"/>
     </row>
     <row r="34" spans="1:26" ht="20.85" customHeight="1">
-      <c r="A34" s="106" t="s">
+      <c r="A34" s="96" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="34" t="s">
@@ -4844,16 +4845,16 @@
         <f>(P35-Q34)/2*(1-0.0003)</f>
         <v>-726.20415820028688</v>
       </c>
-      <c r="T34" s="136"/>
-      <c r="U34" s="115"/>
-      <c r="V34" s="115"/>
-      <c r="W34" s="115"/>
-      <c r="X34" s="137"/>
-      <c r="Y34" s="102"/>
-      <c r="Z34" s="131"/>
+      <c r="T34" s="110"/>
+      <c r="U34" s="111"/>
+      <c r="V34" s="111"/>
+      <c r="W34" s="111"/>
+      <c r="X34" s="112"/>
+      <c r="Y34" s="108"/>
+      <c r="Z34" s="109"/>
     </row>
     <row r="35" spans="1:26" ht="21.3" customHeight="1">
-      <c r="A35" s="120"/>
+      <c r="A35" s="97"/>
       <c r="B35" s="48">
         <f>SQRT(V31*10^6/10^18)*2^96</f>
         <v>4.3829404692999735E+24</v>
@@ -4921,13 +4922,13 @@
         <v>13275.054110200288</v>
       </c>
       <c r="S35" s="56"/>
-      <c r="T35" s="138"/>
-      <c r="U35" s="139"/>
-      <c r="V35" s="139"/>
-      <c r="W35" s="139"/>
-      <c r="X35" s="140"/>
-      <c r="Y35" s="141"/>
-      <c r="Z35" s="142"/>
+      <c r="T35" s="113"/>
+      <c r="U35" s="114"/>
+      <c r="V35" s="114"/>
+      <c r="W35" s="114"/>
+      <c r="X35" s="115"/>
+      <c r="Y35" s="116"/>
+      <c r="Z35" s="117"/>
     </row>
     <row r="36" spans="1:26" ht="21.3" customHeight="1">
       <c r="A36" s="57"/>
@@ -4986,65 +4987,65 @@
       <c r="Z37" s="59"/>
     </row>
     <row r="38" spans="1:26" ht="9.4499999999999993" customHeight="1">
-      <c r="A38" s="125"/>
-      <c r="B38" s="127" t="s">
+      <c r="A38" s="98"/>
+      <c r="B38" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="111"/>
-      <c r="D38" s="111"/>
-      <c r="E38" s="111"/>
-      <c r="F38" s="111"/>
-      <c r="G38" s="111"/>
-      <c r="H38" s="111"/>
-      <c r="I38" s="111"/>
-      <c r="J38" s="111"/>
-      <c r="K38" s="111"/>
-      <c r="L38" s="111"/>
-      <c r="M38" s="111"/>
-      <c r="N38" s="111"/>
-      <c r="O38" s="111"/>
-      <c r="P38" s="111"/>
-      <c r="Q38" s="111"/>
-      <c r="R38" s="111"/>
-      <c r="S38" s="111"/>
-      <c r="T38" s="111"/>
-      <c r="U38" s="111"/>
-      <c r="V38" s="111"/>
-      <c r="W38" s="111"/>
-      <c r="X38" s="111"/>
-      <c r="Y38" s="128"/>
-      <c r="Z38" s="129"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="120"/>
+      <c r="E38" s="120"/>
+      <c r="F38" s="120"/>
+      <c r="G38" s="120"/>
+      <c r="H38" s="120"/>
+      <c r="I38" s="120"/>
+      <c r="J38" s="120"/>
+      <c r="K38" s="120"/>
+      <c r="L38" s="120"/>
+      <c r="M38" s="120"/>
+      <c r="N38" s="120"/>
+      <c r="O38" s="120"/>
+      <c r="P38" s="120"/>
+      <c r="Q38" s="120"/>
+      <c r="R38" s="120"/>
+      <c r="S38" s="120"/>
+      <c r="T38" s="120"/>
+      <c r="U38" s="120"/>
+      <c r="V38" s="120"/>
+      <c r="W38" s="120"/>
+      <c r="X38" s="120"/>
+      <c r="Y38" s="125"/>
+      <c r="Z38" s="126"/>
     </row>
     <row r="39" spans="1:26" ht="21.9" customHeight="1">
-      <c r="A39" s="126"/>
-      <c r="B39" s="108"/>
-      <c r="C39" s="108"/>
-      <c r="D39" s="108"/>
-      <c r="E39" s="115"/>
-      <c r="F39" s="115"/>
-      <c r="G39" s="115"/>
-      <c r="H39" s="115"/>
-      <c r="I39" s="115"/>
-      <c r="J39" s="115"/>
-      <c r="K39" s="115"/>
-      <c r="L39" s="115"/>
-      <c r="M39" s="115"/>
-      <c r="N39" s="115"/>
-      <c r="O39" s="115"/>
-      <c r="P39" s="115"/>
-      <c r="Q39" s="115"/>
-      <c r="R39" s="115"/>
-      <c r="S39" s="115"/>
-      <c r="T39" s="115"/>
-      <c r="U39" s="115"/>
-      <c r="V39" s="108"/>
-      <c r="W39" s="108"/>
-      <c r="X39" s="108"/>
-      <c r="Y39" s="111"/>
-      <c r="Z39" s="130"/>
+      <c r="A39" s="99"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="103"/>
+      <c r="D39" s="103"/>
+      <c r="E39" s="111"/>
+      <c r="F39" s="111"/>
+      <c r="G39" s="111"/>
+      <c r="H39" s="111"/>
+      <c r="I39" s="111"/>
+      <c r="J39" s="111"/>
+      <c r="K39" s="111"/>
+      <c r="L39" s="111"/>
+      <c r="M39" s="111"/>
+      <c r="N39" s="111"/>
+      <c r="O39" s="111"/>
+      <c r="P39" s="111"/>
+      <c r="Q39" s="111"/>
+      <c r="R39" s="111"/>
+      <c r="S39" s="111"/>
+      <c r="T39" s="111"/>
+      <c r="U39" s="111"/>
+      <c r="V39" s="103"/>
+      <c r="W39" s="103"/>
+      <c r="X39" s="103"/>
+      <c r="Y39" s="120"/>
+      <c r="Z39" s="127"/>
     </row>
     <row r="40" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A40" s="123"/>
+      <c r="A40" s="100"/>
       <c r="B40" s="22" t="s">
         <v>4</v>
       </c>
@@ -5056,23 +5057,23 @@
         <f>B42/0.81</f>
         <v>3778.2175195446539</v>
       </c>
-      <c r="E40" s="107"/>
-      <c r="F40" s="108"/>
-      <c r="G40" s="108"/>
-      <c r="H40" s="108"/>
-      <c r="I40" s="108"/>
-      <c r="J40" s="108"/>
-      <c r="K40" s="108"/>
-      <c r="L40" s="108"/>
-      <c r="M40" s="108"/>
-      <c r="N40" s="108"/>
-      <c r="O40" s="108"/>
-      <c r="P40" s="108"/>
-      <c r="Q40" s="108"/>
-      <c r="R40" s="108"/>
-      <c r="S40" s="108"/>
-      <c r="T40" s="108"/>
-      <c r="U40" s="109"/>
+      <c r="E40" s="102"/>
+      <c r="F40" s="103"/>
+      <c r="G40" s="103"/>
+      <c r="H40" s="103"/>
+      <c r="I40" s="103"/>
+      <c r="J40" s="103"/>
+      <c r="K40" s="103"/>
+      <c r="L40" s="103"/>
+      <c r="M40" s="103"/>
+      <c r="N40" s="103"/>
+      <c r="O40" s="103"/>
+      <c r="P40" s="103"/>
+      <c r="Q40" s="103"/>
+      <c r="R40" s="103"/>
+      <c r="S40" s="103"/>
+      <c r="T40" s="103"/>
+      <c r="U40" s="104"/>
       <c r="V40" s="22" t="s">
         <v>4</v>
       </c>
@@ -5088,7 +5089,7 @@
       <c r="Z40" s="119"/>
     </row>
     <row r="41" spans="1:26" ht="23.85" customHeight="1">
-      <c r="A41" s="123"/>
+      <c r="A41" s="100"/>
       <c r="B41" s="25" t="s">
         <v>5</v>
       </c>
@@ -5166,7 +5167,7 @@
       </c>
     </row>
     <row r="42" spans="1:26" ht="40.799999999999997" customHeight="1">
-      <c r="A42" s="124"/>
+      <c r="A42" s="101"/>
       <c r="B42" s="30">
         <f t="shared" si="1"/>
         <v>3060.3561908311699</v>
@@ -5266,7 +5267,7 @@
       </c>
     </row>
     <row r="43" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A43" s="106" t="s">
+      <c r="A43" s="96" t="s">
         <v>28</v>
       </c>
       <c r="B43" s="34" t="s">
@@ -5308,23 +5309,23 @@
       <c r="N43" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O43" s="103" t="s">
+      <c r="O43" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="P43" s="104"/>
-      <c r="Q43" s="104"/>
-      <c r="R43" s="105"/>
-      <c r="S43" s="102"/>
-      <c r="T43" s="134"/>
-      <c r="U43" s="116"/>
-      <c r="V43" s="116"/>
-      <c r="W43" s="116"/>
-      <c r="X43" s="135"/>
-      <c r="Y43" s="102"/>
-      <c r="Z43" s="131"/>
+      <c r="P43" s="130"/>
+      <c r="Q43" s="130"/>
+      <c r="R43" s="131"/>
+      <c r="S43" s="108"/>
+      <c r="T43" s="105"/>
+      <c r="U43" s="106"/>
+      <c r="V43" s="106"/>
+      <c r="W43" s="106"/>
+      <c r="X43" s="107"/>
+      <c r="Y43" s="108"/>
+      <c r="Z43" s="109"/>
     </row>
     <row r="44" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A44" s="106"/>
+      <c r="A44" s="96"/>
       <c r="B44" s="39">
         <f>SQRT(B42*10^6/10^18)*2^96</f>
         <v>4.3829404691790772E+24</v>
@@ -5376,27 +5377,27 @@
         <f>M44-(0.1*E44)*B44</f>
         <v>1.7108169422649108E+43</v>
       </c>
-      <c r="O44" s="101" t="s">
+      <c r="O44" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="P44" s="102"/>
-      <c r="Q44" s="101" t="s">
+      <c r="P44" s="108"/>
+      <c r="Q44" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="R44" s="102"/>
+      <c r="R44" s="108"/>
       <c r="S44" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="T44" s="136"/>
-      <c r="U44" s="115"/>
-      <c r="V44" s="115"/>
-      <c r="W44" s="115"/>
-      <c r="X44" s="137"/>
-      <c r="Y44" s="102"/>
-      <c r="Z44" s="131"/>
+      <c r="T44" s="110"/>
+      <c r="U44" s="111"/>
+      <c r="V44" s="111"/>
+      <c r="W44" s="111"/>
+      <c r="X44" s="112"/>
+      <c r="Y44" s="108"/>
+      <c r="Z44" s="109"/>
     </row>
     <row r="45" spans="1:26" ht="20.85" customHeight="1">
-      <c r="A45" s="106" t="s">
+      <c r="A45" s="96" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="34" t="s">
@@ -5457,16 +5458,16 @@
         <f>(P46-Q45)/2*(1-0.0003)</f>
         <v>-9.6591083419882153</v>
       </c>
-      <c r="T45" s="136"/>
-      <c r="U45" s="115"/>
-      <c r="V45" s="115"/>
-      <c r="W45" s="115"/>
-      <c r="X45" s="137"/>
-      <c r="Y45" s="102"/>
-      <c r="Z45" s="131"/>
+      <c r="T45" s="110"/>
+      <c r="U45" s="111"/>
+      <c r="V45" s="111"/>
+      <c r="W45" s="111"/>
+      <c r="X45" s="112"/>
+      <c r="Y45" s="108"/>
+      <c r="Z45" s="109"/>
     </row>
     <row r="46" spans="1:26" ht="21.3" customHeight="1">
-      <c r="A46" s="120"/>
+      <c r="A46" s="97"/>
       <c r="B46" s="48">
         <f>SQRT(V42*10^6/10^18)*2^96</f>
         <v>4.3829404692999735E+24</v>
@@ -5534,13 +5535,13 @@
         <v>13263.284455341987</v>
       </c>
       <c r="S46" s="56"/>
-      <c r="T46" s="138"/>
-      <c r="U46" s="139"/>
-      <c r="V46" s="139"/>
-      <c r="W46" s="139"/>
-      <c r="X46" s="140"/>
-      <c r="Y46" s="141"/>
-      <c r="Z46" s="142"/>
+      <c r="T46" s="113"/>
+      <c r="U46" s="114"/>
+      <c r="V46" s="114"/>
+      <c r="W46" s="114"/>
+      <c r="X46" s="115"/>
+      <c r="Y46" s="116"/>
+      <c r="Z46" s="117"/>
     </row>
     <row r="47" spans="1:26" ht="21.3" customHeight="1">
       <c r="A47" s="57"/>
@@ -5599,65 +5600,65 @@
       <c r="Z48" s="59"/>
     </row>
     <row r="49" spans="1:26" ht="9.4499999999999993" customHeight="1">
-      <c r="A49" s="125"/>
-      <c r="B49" s="127" t="s">
+      <c r="A49" s="98"/>
+      <c r="B49" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="111"/>
-      <c r="D49" s="111"/>
-      <c r="E49" s="111"/>
-      <c r="F49" s="111"/>
-      <c r="G49" s="111"/>
-      <c r="H49" s="111"/>
-      <c r="I49" s="111"/>
-      <c r="J49" s="111"/>
-      <c r="K49" s="111"/>
-      <c r="L49" s="111"/>
-      <c r="M49" s="111"/>
-      <c r="N49" s="111"/>
-      <c r="O49" s="111"/>
-      <c r="P49" s="111"/>
-      <c r="Q49" s="111"/>
-      <c r="R49" s="111"/>
-      <c r="S49" s="111"/>
-      <c r="T49" s="111"/>
-      <c r="U49" s="111"/>
-      <c r="V49" s="111"/>
-      <c r="W49" s="111"/>
-      <c r="X49" s="111"/>
-      <c r="Y49" s="128"/>
-      <c r="Z49" s="129"/>
+      <c r="C49" s="120"/>
+      <c r="D49" s="120"/>
+      <c r="E49" s="120"/>
+      <c r="F49" s="120"/>
+      <c r="G49" s="120"/>
+      <c r="H49" s="120"/>
+      <c r="I49" s="120"/>
+      <c r="J49" s="120"/>
+      <c r="K49" s="120"/>
+      <c r="L49" s="120"/>
+      <c r="M49" s="120"/>
+      <c r="N49" s="120"/>
+      <c r="O49" s="120"/>
+      <c r="P49" s="120"/>
+      <c r="Q49" s="120"/>
+      <c r="R49" s="120"/>
+      <c r="S49" s="120"/>
+      <c r="T49" s="120"/>
+      <c r="U49" s="120"/>
+      <c r="V49" s="120"/>
+      <c r="W49" s="120"/>
+      <c r="X49" s="120"/>
+      <c r="Y49" s="125"/>
+      <c r="Z49" s="126"/>
     </row>
     <row r="50" spans="1:26" ht="21.9" customHeight="1">
-      <c r="A50" s="126"/>
-      <c r="B50" s="108"/>
-      <c r="C50" s="108"/>
-      <c r="D50" s="108"/>
-      <c r="E50" s="115"/>
-      <c r="F50" s="115"/>
-      <c r="G50" s="115"/>
-      <c r="H50" s="115"/>
-      <c r="I50" s="115"/>
-      <c r="J50" s="115"/>
-      <c r="K50" s="115"/>
-      <c r="L50" s="115"/>
-      <c r="M50" s="115"/>
-      <c r="N50" s="115"/>
-      <c r="O50" s="115"/>
-      <c r="P50" s="115"/>
-      <c r="Q50" s="115"/>
-      <c r="R50" s="115"/>
-      <c r="S50" s="115"/>
-      <c r="T50" s="115"/>
-      <c r="U50" s="115"/>
-      <c r="V50" s="108"/>
-      <c r="W50" s="108"/>
-      <c r="X50" s="108"/>
-      <c r="Y50" s="111"/>
-      <c r="Z50" s="130"/>
+      <c r="A50" s="99"/>
+      <c r="B50" s="103"/>
+      <c r="C50" s="103"/>
+      <c r="D50" s="103"/>
+      <c r="E50" s="111"/>
+      <c r="F50" s="111"/>
+      <c r="G50" s="111"/>
+      <c r="H50" s="111"/>
+      <c r="I50" s="111"/>
+      <c r="J50" s="111"/>
+      <c r="K50" s="111"/>
+      <c r="L50" s="111"/>
+      <c r="M50" s="111"/>
+      <c r="N50" s="111"/>
+      <c r="O50" s="111"/>
+      <c r="P50" s="111"/>
+      <c r="Q50" s="111"/>
+      <c r="R50" s="111"/>
+      <c r="S50" s="111"/>
+      <c r="T50" s="111"/>
+      <c r="U50" s="111"/>
+      <c r="V50" s="103"/>
+      <c r="W50" s="103"/>
+      <c r="X50" s="103"/>
+      <c r="Y50" s="120"/>
+      <c r="Z50" s="127"/>
     </row>
     <row r="51" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A51" s="123"/>
+      <c r="A51" s="100"/>
       <c r="B51" s="22" t="s">
         <v>4</v>
       </c>
@@ -5669,39 +5670,39 @@
         <f>B53/0.81</f>
         <v>3778.2175195446539</v>
       </c>
-      <c r="E51" s="107"/>
-      <c r="F51" s="108"/>
-      <c r="G51" s="108"/>
-      <c r="H51" s="108"/>
-      <c r="I51" s="108"/>
-      <c r="J51" s="108"/>
-      <c r="K51" s="108"/>
-      <c r="L51" s="108"/>
-      <c r="M51" s="108"/>
-      <c r="N51" s="108"/>
-      <c r="O51" s="108"/>
-      <c r="P51" s="108"/>
-      <c r="Q51" s="108"/>
-      <c r="R51" s="108"/>
-      <c r="S51" s="108"/>
-      <c r="T51" s="108"/>
-      <c r="U51" s="109"/>
+      <c r="E51" s="102"/>
+      <c r="F51" s="103"/>
+      <c r="G51" s="103"/>
+      <c r="H51" s="103"/>
+      <c r="I51" s="103"/>
+      <c r="J51" s="103"/>
+      <c r="K51" s="103"/>
+      <c r="L51" s="103"/>
+      <c r="M51" s="103"/>
+      <c r="N51" s="103"/>
+      <c r="O51" s="103"/>
+      <c r="P51" s="103"/>
+      <c r="Q51" s="103"/>
+      <c r="R51" s="103"/>
+      <c r="S51" s="103"/>
+      <c r="T51" s="103"/>
+      <c r="U51" s="104"/>
       <c r="V51" s="22" t="s">
         <v>4</v>
       </c>
       <c r="W51" s="23">
         <f>0.81*V53</f>
-        <v>1267.1266938300002</v>
+        <v>3593.4549453</v>
       </c>
       <c r="X51" s="24">
         <f>V53/0.81</f>
-        <v>1931.3011641975309</v>
+        <v>5476.9927530864197</v>
       </c>
       <c r="Y51" s="118"/>
       <c r="Z51" s="119"/>
     </row>
     <row r="52" spans="1:26" ht="23.85" customHeight="1">
-      <c r="A52" s="123"/>
+      <c r="A52" s="100"/>
       <c r="B52" s="25" t="s">
         <v>5</v>
       </c>
@@ -5778,8 +5779,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="40.65" customHeight="1">
-      <c r="A53" s="124"/>
+    <row r="53" spans="1:26" ht="40.65" customHeight="1" thickBot="1">
+      <c r="A53" s="101"/>
       <c r="B53" s="30">
         <f t="shared" si="1"/>
         <v>3060.3561908311699</v>
@@ -5833,54 +5834,54 @@
         <v>1127.69398</v>
       </c>
       <c r="O53" s="31">
-        <v>1564.3539430000001</v>
+        <v>4436.3641299999999</v>
       </c>
       <c r="P53" s="31">
         <f>IF(S56&lt;0,ABS(S56)/O53,0)</f>
-        <v>0</v>
+        <v>0.21415488411437469</v>
       </c>
       <c r="Q53" s="31">
         <f>IF(S56&gt;0,S56,0)</f>
-        <v>3265.8246085298442</v>
+        <v>0</v>
       </c>
       <c r="R53" s="31">
         <f>R56</f>
-        <v>5.024380399238205</v>
+        <v>2.7225748123251452</v>
       </c>
       <c r="S53" s="31">
         <f>R57</f>
-        <v>7861.8693714701558</v>
+        <v>12077.763026149318</v>
       </c>
       <c r="T53" s="31">
         <f>R53*$B$3</f>
-        <v>0.50243803992382052</v>
+        <v>0.27225748123251453</v>
       </c>
       <c r="U53" s="31">
         <f>S53*$B$3</f>
-        <v>786.18693714701567</v>
+        <v>1207.7763026149319</v>
       </c>
       <c r="V53" s="31">
-        <v>1564.3539430000001</v>
+        <v>4436.3641299999999</v>
       </c>
       <c r="W53" s="31">
         <f>IF((LOG(1/(C57*C57*10^12/2^96/2^96)*10^12,1.0001)-FLOOR(LOG(1/(C57*C57*10^12/2^96/2^96)*10^12,1.0001)/60,1)*60)&gt;(CEILING(LOG(1/(C57*C57*10^12/2^96/2^96)*10^12,1.0001)/60,1)*60)-(LOG(1/(C57*C57*10^12/2^96/2^96)*10^12,1.0001)),CEILING(LOG(1/(C57*C57*10^12/2^96/2^96)*10^12,1.0001)/60,1)*60,FLOOR(LOG(1/(C57*C57*10^12/2^96/2^96)*10^12,1.0001)/60,1)*60)</f>
-        <v>204900</v>
+        <v>194460</v>
       </c>
       <c r="X53" s="31">
         <f>IF((LOG(1/(D57*D57*10^12/2^96/2^96)*10^12,1.0001)-FLOOR(LOG(1/(D57*D57*10^12/2^96/2^96)*10^12,1.0001)/60,1)*60)&gt;(CEILING(LOG(1/(D57*D57*10^12/2^96/2^96)*10^12,1.0001)/60,1)*60)-(LOG(1/(D57*D57*10^12/2^96/2^96)*10^12,1.0001)),CEILING(LOG(1/(D57*D57*10^12/2^96/2^96)*10^12,1.0001)/60,1)*60,FLOOR(LOG(1/(D57*D57*10^12/2^96/2^96)*10^12,1.0001)/60,1)*60)</f>
-        <v>200640</v>
+        <v>190260</v>
       </c>
       <c r="Y53" s="32">
         <f>(G57/T53)-1</f>
-        <v>9.3327296662113479E-3</v>
+        <v>-1.0578861070834944E-2</v>
       </c>
       <c r="Z53" s="33">
         <f>(H57/U53)-1</f>
-        <v>1.0818413269359395E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A54" s="106" t="s">
+        <v>3.9413521850302224E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A54" s="96" t="s">
         <v>28</v>
       </c>
       <c r="B54" s="34" t="s">
@@ -5922,23 +5923,23 @@
       <c r="N54" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O54" s="103" t="s">
+      <c r="O54" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="P54" s="104"/>
-      <c r="Q54" s="104"/>
-      <c r="R54" s="105"/>
-      <c r="S54" s="102"/>
-      <c r="T54" s="134"/>
-      <c r="U54" s="116"/>
-      <c r="V54" s="116"/>
-      <c r="W54" s="116"/>
-      <c r="X54" s="135"/>
-      <c r="Y54" s="102"/>
-      <c r="Z54" s="131"/>
+      <c r="P54" s="130"/>
+      <c r="Q54" s="130"/>
+      <c r="R54" s="131"/>
+      <c r="S54" s="108"/>
+      <c r="T54" s="105"/>
+      <c r="U54" s="106"/>
+      <c r="V54" s="106"/>
+      <c r="W54" s="106"/>
+      <c r="X54" s="107"/>
+      <c r="Y54" s="108"/>
+      <c r="Z54" s="109"/>
     </row>
     <row r="55" spans="1:26" ht="21.75" customHeight="1">
-      <c r="A55" s="106"/>
+      <c r="A55" s="96"/>
       <c r="B55" s="39">
         <f>SQRT(B53*10^6/10^18)*2^96</f>
         <v>4.3829404691790772E+24</v>
@@ -5990,27 +5991,27 @@
         <f>M55-(0.1*E55)*B55</f>
         <v>1.2889378916075946E+43</v>
       </c>
-      <c r="O55" s="101" t="s">
+      <c r="O55" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="P55" s="102"/>
-      <c r="Q55" s="101" t="s">
+      <c r="P55" s="108"/>
+      <c r="Q55" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="R55" s="102"/>
+      <c r="R55" s="108"/>
       <c r="S55" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="T55" s="136"/>
-      <c r="U55" s="115"/>
-      <c r="V55" s="115"/>
-      <c r="W55" s="115"/>
-      <c r="X55" s="137"/>
-      <c r="Y55" s="102"/>
-      <c r="Z55" s="131"/>
+      <c r="T55" s="110"/>
+      <c r="U55" s="111"/>
+      <c r="V55" s="111"/>
+      <c r="W55" s="111"/>
+      <c r="X55" s="112"/>
+      <c r="Y55" s="108"/>
+      <c r="Z55" s="109"/>
     </row>
     <row r="56" spans="1:26" ht="32.85" customHeight="1">
-      <c r="A56" s="106" t="s">
+      <c r="A56" s="96" t="s">
         <v>46</v>
       </c>
       <c r="B56" s="34" t="s">
@@ -6061,76 +6062,76 @@
       </c>
       <c r="Q56" s="46">
         <f>P56*O53</f>
-        <v>4594.0846801503567</v>
+        <v>13028.402284790074</v>
       </c>
       <c r="R56" s="47">
         <f>P56+(S56/O53)</f>
-        <v>5.024380399238205</v>
+        <v>2.7225748123251452</v>
       </c>
       <c r="S56" s="47">
         <f>(P57-Q56)/2*(1-0.0003)</f>
-        <v>3265.8246085298442</v>
-      </c>
-      <c r="T56" s="136"/>
-      <c r="U56" s="115"/>
-      <c r="V56" s="115"/>
-      <c r="W56" s="115"/>
-      <c r="X56" s="137"/>
-      <c r="Y56" s="102"/>
-      <c r="Z56" s="131"/>
+        <v>-950.06904614931864</v>
+      </c>
+      <c r="T56" s="110"/>
+      <c r="U56" s="111"/>
+      <c r="V56" s="111"/>
+      <c r="W56" s="111"/>
+      <c r="X56" s="112"/>
+      <c r="Y56" s="108"/>
+      <c r="Z56" s="109"/>
     </row>
     <row r="57" spans="1:26" ht="21.3" customHeight="1">
-      <c r="A57" s="120"/>
+      <c r="A57" s="97"/>
       <c r="B57" s="48">
         <f>SQRT(V53*10^6/10^18)*2^96</f>
-        <v>3.1336255121447264E+24</v>
+        <v>5.2770739031427465E+24</v>
       </c>
       <c r="C57" s="49">
         <f>B57-$B$3*F57*POWER(2,96)/L57</f>
-        <v>2.8201848154299569E+24</v>
+        <v>4.7493665128284719E+24</v>
       </c>
       <c r="D57" s="49">
         <f>M57*B57/N57</f>
-        <v>3.481806124605251E+24</v>
+        <v>5.8634462061181069E+24</v>
       </c>
       <c r="E57" s="49">
         <f>R53*10^18</f>
-        <v>5.0243803992382054E+18</v>
+        <v>2.7225748123251451E+18</v>
       </c>
       <c r="F57" s="49">
         <f>S53*10^6</f>
-        <v>7861869371.4701557</v>
+        <v>12077763026.149317</v>
       </c>
       <c r="G57" s="50">
         <f>(M57-(M57*B57)/(SQRT(1/(1.0001^X53)*2^96*2^96/10^6)*10^3))/B57/10^18</f>
-        <v>0.50712715832445066</v>
+        <v>0.2693773071630603</v>
       </c>
       <c r="H57" s="50">
         <f>(B57-(SQRT(1/(1.0001^W53)*2^96*2^96)))*L57/POWER(2,96)/10^6</f>
-        <v>794.69223234004392</v>
+        <v>1212.536574384271</v>
       </c>
       <c r="I57" s="49">
         <v>9.9999999999999997E+98</v>
       </c>
       <c r="J57" s="49">
         <f>(E57)*(B57*I57)/POWER(2,96)/(I57-B57)</f>
-        <v>198723864117612</v>
+        <v>181339917972830.53</v>
       </c>
       <c r="K57" s="49">
         <f>(F57)*POWER(2,96)/(B57-0)</f>
-        <v>198773421334076.44</v>
+        <v>181331356999691.19</v>
       </c>
       <c r="L57" s="49">
         <f>MIN(J57,K57)</f>
-        <v>198723864117612</v>
+        <v>181331356999691.19</v>
       </c>
       <c r="M57" s="49">
         <f>L57*POWER(2,96)</f>
-        <v>1.5744526601772747E+43</v>
+        <v>1.4366550221303618E+43</v>
       </c>
       <c r="N57" s="51">
         <f>M57-(0.1*E57)*B57</f>
-        <v>1.4170073941595473E+43</v>
+        <v>1.2929827372156139E+43</v>
       </c>
       <c r="O57" s="52" t="s">
         <v>49</v>
@@ -6141,20 +6142,20 @@
       </c>
       <c r="Q57" s="54">
         <f>P57/O53</f>
-        <v>7.1132840683484631</v>
+        <v>2.5082913967208547</v>
       </c>
       <c r="R57" s="55">
         <f>P57-S56</f>
-        <v>7861.8693714701558</v>
+        <v>12077.763026149318</v>
       </c>
       <c r="S57" s="56"/>
-      <c r="T57" s="138"/>
-      <c r="U57" s="139"/>
-      <c r="V57" s="139"/>
-      <c r="W57" s="139"/>
-      <c r="X57" s="140"/>
-      <c r="Y57" s="141"/>
-      <c r="Z57" s="142"/>
+      <c r="T57" s="113"/>
+      <c r="U57" s="114"/>
+      <c r="V57" s="114"/>
+      <c r="W57" s="114"/>
+      <c r="X57" s="115"/>
+      <c r="Y57" s="116"/>
+      <c r="Z57" s="117"/>
     </row>
     <row r="58" spans="1:26" ht="21.3" customHeight="1">
       <c r="A58" s="57"/>
@@ -6213,65 +6214,65 @@
       <c r="Z59" s="67"/>
     </row>
     <row r="60" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A60" s="125"/>
+      <c r="A60" s="98"/>
       <c r="B60" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="116"/>
-      <c r="D60" s="116"/>
-      <c r="E60" s="116"/>
-      <c r="F60" s="116"/>
-      <c r="G60" s="116"/>
-      <c r="H60" s="116"/>
-      <c r="I60" s="116"/>
-      <c r="J60" s="116"/>
-      <c r="K60" s="116"/>
-      <c r="L60" s="116"/>
-      <c r="M60" s="116"/>
-      <c r="N60" s="116"/>
-      <c r="O60" s="116"/>
-      <c r="P60" s="116"/>
-      <c r="Q60" s="116"/>
-      <c r="R60" s="116"/>
-      <c r="S60" s="116"/>
-      <c r="T60" s="116"/>
-      <c r="U60" s="116"/>
-      <c r="V60" s="116"/>
-      <c r="W60" s="116"/>
-      <c r="X60" s="116"/>
-      <c r="Y60" s="104"/>
+      <c r="C60" s="106"/>
+      <c r="D60" s="106"/>
+      <c r="E60" s="106"/>
+      <c r="F60" s="106"/>
+      <c r="G60" s="106"/>
+      <c r="H60" s="106"/>
+      <c r="I60" s="106"/>
+      <c r="J60" s="106"/>
+      <c r="K60" s="106"/>
+      <c r="L60" s="106"/>
+      <c r="M60" s="106"/>
+      <c r="N60" s="106"/>
+      <c r="O60" s="106"/>
+      <c r="P60" s="106"/>
+      <c r="Q60" s="106"/>
+      <c r="R60" s="106"/>
+      <c r="S60" s="106"/>
+      <c r="T60" s="106"/>
+      <c r="U60" s="106"/>
+      <c r="V60" s="106"/>
+      <c r="W60" s="106"/>
+      <c r="X60" s="106"/>
+      <c r="Y60" s="130"/>
       <c r="Z60" s="133"/>
     </row>
     <row r="61" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A61" s="126"/>
-      <c r="B61" s="108"/>
-      <c r="C61" s="108"/>
-      <c r="D61" s="108"/>
-      <c r="E61" s="115"/>
-      <c r="F61" s="115"/>
-      <c r="G61" s="115"/>
-      <c r="H61" s="115"/>
-      <c r="I61" s="115"/>
-      <c r="J61" s="115"/>
-      <c r="K61" s="115"/>
-      <c r="L61" s="115"/>
-      <c r="M61" s="115"/>
-      <c r="N61" s="115"/>
-      <c r="O61" s="115"/>
-      <c r="P61" s="115"/>
-      <c r="Q61" s="115"/>
-      <c r="R61" s="115"/>
-      <c r="S61" s="115"/>
-      <c r="T61" s="115"/>
-      <c r="U61" s="115"/>
-      <c r="V61" s="108"/>
-      <c r="W61" s="108"/>
-      <c r="X61" s="108"/>
-      <c r="Y61" s="116"/>
-      <c r="Z61" s="117"/>
+      <c r="A61" s="99"/>
+      <c r="B61" s="103"/>
+      <c r="C61" s="103"/>
+      <c r="D61" s="103"/>
+      <c r="E61" s="111"/>
+      <c r="F61" s="111"/>
+      <c r="G61" s="111"/>
+      <c r="H61" s="111"/>
+      <c r="I61" s="111"/>
+      <c r="J61" s="111"/>
+      <c r="K61" s="111"/>
+      <c r="L61" s="111"/>
+      <c r="M61" s="111"/>
+      <c r="N61" s="111"/>
+      <c r="O61" s="111"/>
+      <c r="P61" s="111"/>
+      <c r="Q61" s="111"/>
+      <c r="R61" s="111"/>
+      <c r="S61" s="111"/>
+      <c r="T61" s="111"/>
+      <c r="U61" s="111"/>
+      <c r="V61" s="103"/>
+      <c r="W61" s="103"/>
+      <c r="X61" s="103"/>
+      <c r="Y61" s="106"/>
+      <c r="Z61" s="134"/>
     </row>
     <row r="62" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A62" s="123"/>
+      <c r="A62" s="100"/>
       <c r="B62" s="22" t="s">
         <v>4</v>
       </c>
@@ -6283,23 +6284,23 @@
         <f>B64/0.81</f>
         <v>3778.1061728382715</v>
       </c>
-      <c r="E62" s="107"/>
-      <c r="F62" s="108"/>
-      <c r="G62" s="108"/>
-      <c r="H62" s="108"/>
-      <c r="I62" s="108"/>
-      <c r="J62" s="108"/>
-      <c r="K62" s="108"/>
-      <c r="L62" s="108"/>
-      <c r="M62" s="108"/>
-      <c r="N62" s="108"/>
-      <c r="O62" s="108"/>
-      <c r="P62" s="108"/>
-      <c r="Q62" s="108"/>
-      <c r="R62" s="108"/>
-      <c r="S62" s="108"/>
-      <c r="T62" s="108"/>
-      <c r="U62" s="109"/>
+      <c r="E62" s="102"/>
+      <c r="F62" s="103"/>
+      <c r="G62" s="103"/>
+      <c r="H62" s="103"/>
+      <c r="I62" s="103"/>
+      <c r="J62" s="103"/>
+      <c r="K62" s="103"/>
+      <c r="L62" s="103"/>
+      <c r="M62" s="103"/>
+      <c r="N62" s="103"/>
+      <c r="O62" s="103"/>
+      <c r="P62" s="103"/>
+      <c r="Q62" s="103"/>
+      <c r="R62" s="103"/>
+      <c r="S62" s="103"/>
+      <c r="T62" s="103"/>
+      <c r="U62" s="104"/>
       <c r="V62" s="22" t="s">
         <v>4</v>
       </c>
@@ -6315,7 +6316,7 @@
       <c r="Z62" s="119"/>
     </row>
     <row r="63" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A63" s="123"/>
+      <c r="A63" s="100"/>
       <c r="B63" s="68" t="s">
         <v>5</v>
       </c>
@@ -6393,7 +6394,7 @@
       </c>
     </row>
     <row r="64" spans="1:26" ht="36" customHeight="1">
-      <c r="A64" s="124"/>
+      <c r="A64" s="101"/>
       <c r="B64" s="69">
         <f t="shared" ref="B64:D70" si="3">3060.265999999</f>
         <v>3060.2659999990001</v>
@@ -6492,7 +6493,7 @@
       </c>
     </row>
     <row r="65" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A65" s="106" t="s">
+      <c r="A65" s="96" t="s">
         <v>28</v>
       </c>
       <c r="B65" s="34" t="s">
@@ -6534,23 +6535,23 @@
       <c r="N65" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O65" s="103" t="s">
+      <c r="O65" s="129" t="s">
         <v>42</v>
       </c>
-      <c r="P65" s="104"/>
-      <c r="Q65" s="104"/>
-      <c r="R65" s="105"/>
-      <c r="S65" s="131"/>
-      <c r="T65" s="125"/>
-      <c r="U65" s="111"/>
-      <c r="V65" s="111"/>
-      <c r="W65" s="116"/>
-      <c r="X65" s="135"/>
-      <c r="Y65" s="143"/>
-      <c r="Z65" s="144"/>
+      <c r="P65" s="130"/>
+      <c r="Q65" s="130"/>
+      <c r="R65" s="131"/>
+      <c r="S65" s="109"/>
+      <c r="T65" s="98"/>
+      <c r="U65" s="120"/>
+      <c r="V65" s="120"/>
+      <c r="W65" s="106"/>
+      <c r="X65" s="107"/>
+      <c r="Y65" s="121"/>
+      <c r="Z65" s="122"/>
     </row>
     <row r="66" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A66" s="106"/>
+      <c r="A66" s="96"/>
       <c r="B66" s="39">
         <f>SQRT(B64*10^6/10^18)*2^96</f>
         <v>4.382875884546422E+24</v>
@@ -6602,27 +6603,27 @@
         <f>M66-($B$3*E66)*B66</f>
         <v>1.2889611060943387E+43</v>
       </c>
-      <c r="O66" s="101" t="s">
+      <c r="O66" s="128" t="s">
         <v>43</v>
       </c>
-      <c r="P66" s="102"/>
-      <c r="Q66" s="101" t="s">
+      <c r="P66" s="108"/>
+      <c r="Q66" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="R66" s="102"/>
+      <c r="R66" s="108"/>
       <c r="S66" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="T66" s="126"/>
-      <c r="U66" s="115"/>
-      <c r="V66" s="115"/>
-      <c r="W66" s="115"/>
-      <c r="X66" s="137"/>
-      <c r="Y66" s="102"/>
-      <c r="Z66" s="131"/>
+      <c r="T66" s="99"/>
+      <c r="U66" s="111"/>
+      <c r="V66" s="111"/>
+      <c r="W66" s="111"/>
+      <c r="X66" s="112"/>
+      <c r="Y66" s="108"/>
+      <c r="Z66" s="109"/>
     </row>
     <row r="67" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A67" s="106" t="s">
+      <c r="A67" s="96" t="s">
         <v>46</v>
       </c>
       <c r="B67" s="34" t="s">
@@ -6683,16 +6684,16 @@
         <f>(P68-Q67)/2*(1-0.0003)</f>
         <v>-0.42613968412199249</v>
       </c>
-      <c r="T67" s="126"/>
-      <c r="U67" s="115"/>
-      <c r="V67" s="115"/>
-      <c r="W67" s="115"/>
-      <c r="X67" s="137"/>
-      <c r="Y67" s="102"/>
-      <c r="Z67" s="131"/>
+      <c r="T67" s="99"/>
+      <c r="U67" s="111"/>
+      <c r="V67" s="111"/>
+      <c r="W67" s="111"/>
+      <c r="X67" s="112"/>
+      <c r="Y67" s="108"/>
+      <c r="Z67" s="109"/>
     </row>
     <row r="68" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A68" s="120"/>
+      <c r="A68" s="97"/>
       <c r="B68" s="48">
         <f>SQRT(V64*10^6/10^18)*2^96</f>
         <v>4.3829404692999735E+24</v>
@@ -6760,13 +6761,13 @@
         <v>10000.426139684121</v>
       </c>
       <c r="S68" s="75"/>
-      <c r="T68" s="145"/>
-      <c r="U68" s="139"/>
-      <c r="V68" s="139"/>
-      <c r="W68" s="139"/>
-      <c r="X68" s="140"/>
-      <c r="Y68" s="141"/>
-      <c r="Z68" s="142"/>
+      <c r="T68" s="123"/>
+      <c r="U68" s="114"/>
+      <c r="V68" s="114"/>
+      <c r="W68" s="114"/>
+      <c r="X68" s="115"/>
+      <c r="Y68" s="116"/>
+      <c r="Z68" s="117"/>
     </row>
     <row r="69" spans="1:26" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="76"/>
@@ -7118,6 +7119,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="O10:S10"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="E7:U7"/>
+    <mergeCell ref="B5:Z6"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="E18:U18"/>
+    <mergeCell ref="E29:U29"/>
+    <mergeCell ref="E40:U40"/>
+    <mergeCell ref="E51:U51"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="O21:S21"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="O32:S32"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="O43:S43"/>
+    <mergeCell ref="B27:Z28"/>
+    <mergeCell ref="B38:Z39"/>
+    <mergeCell ref="B49:Z50"/>
+    <mergeCell ref="O55:P55"/>
+    <mergeCell ref="Q55:R55"/>
+    <mergeCell ref="O54:S54"/>
+    <mergeCell ref="O66:P66"/>
+    <mergeCell ref="Q66:R66"/>
+    <mergeCell ref="O65:S65"/>
+    <mergeCell ref="B60:Z61"/>
     <mergeCell ref="A65:A66"/>
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="A60:A64"/>
@@ -7134,51 +7180,6 @@
     <mergeCell ref="T54:Z57"/>
     <mergeCell ref="T65:Z68"/>
     <mergeCell ref="B16:Z17"/>
-    <mergeCell ref="O55:P55"/>
-    <mergeCell ref="Q55:R55"/>
-    <mergeCell ref="O54:S54"/>
-    <mergeCell ref="O66:P66"/>
-    <mergeCell ref="Q66:R66"/>
-    <mergeCell ref="O65:S65"/>
-    <mergeCell ref="B60:Z61"/>
-    <mergeCell ref="E18:U18"/>
-    <mergeCell ref="E29:U29"/>
-    <mergeCell ref="E40:U40"/>
-    <mergeCell ref="E51:U51"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="O21:S21"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="O32:S32"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="O43:S43"/>
-    <mergeCell ref="B27:Z28"/>
-    <mergeCell ref="B38:Z39"/>
-    <mergeCell ref="B49:Z50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A1:X1"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="O10:S10"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="E7:U7"/>
-    <mergeCell ref="B5:Z6"/>
-    <mergeCell ref="Y7:Z7"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup scale="72" orientation="portrait" r:id="rId1"/>

</xml_diff>